<commit_message>
resolve conflict between MOP:0000591 & MOP:0000713 in RXNO
MOP:0000591 is the correct ID for 'carboxylation' but was wrongly declared with MOP:0000713 in RXNO --> affects subclass RXNO:0000182; copied "has_participant some 'carboxy group'" axiom to MOP:0000591 in MOP and deleted this class in RXNO, also made comments to reflect this change; parent (acylation) was already changed to be a subclass of  "organylation" in 202e2154150a069569a0e2ad8722810b7bde916d
</commit_message>
<xml_diff>
--- a/docs/#27_workfiles/MOP_vs_RXNO.xlsx
+++ b/docs/#27_workfiles/MOP_vs_RXNO.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11372" uniqueCount="7358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11370" uniqueCount="7358">
   <si>
     <t>ID</t>
   </si>
@@ -22084,9 +22084,6 @@
     <t>use MOP version, as its parent is more precise</t>
   </si>
   <si>
-    <t>MOP:0000591 is the correct ID for 'carboxylation' --&gt; affects subclass RXNO:0000182, but copy has participant axiom to MOP:0000591, also make comments to reflect this change; change parent (acylation) to be a subclass of  "organylation" as it is in RXNO and not just a sibling as it is in MOP right now</t>
-  </si>
-  <si>
     <t>"carbonyl oxidation to alkyne" has wrong ID, as this was taken by MOP already, thus needs a new ID to be minted in MOP</t>
   </si>
   <si>
@@ -22172,6 +22169,9 @@
   <si>
     <t xml:space="preserve"> merge MOP:0000708 and RXNO:0000344 and make the latter obsolete
 subsume children according to RXNO:0000344 before its obsoletion and add axiomatization as proposed in rsc-ontologies#27 (comment)</t>
+  </si>
+  <si>
+    <t>MOP:0000591 is the correct ID for 'carboxylation' --&gt; affects subclass RXNO:0000182; copy "has_participant some 'carboxy group'" axiom to MOP:0000591, also make comments to reflect this change; change parent (acylation) to be a subclass of  "organylation" as it is in RXNO and not just a sibling as it is in MOP right now</t>
   </si>
 </sst>
 </file>
@@ -23056,8 +23056,8 @@
   <dimension ref="A1:J3621"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A342" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <pane ySplit="2" topLeftCell="A708" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G716" sqref="G716"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23093,7 +23093,7 @@
         <v>7314</v>
       </c>
       <c r="I1" t="s">
-        <v>7338</v>
+        <v>7337</v>
       </c>
     </row>
     <row r="2" spans="1:9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -23186,11 +23186,11 @@
         <v>15</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="7" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -28561,7 +28561,7 @@
       </c>
       <c r="H342" s="11"/>
       <c r="I342" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="343" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -28972,7 +28972,7 @@
       </c>
       <c r="H367" s="11"/>
       <c r="I367" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="368" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -29063,7 +29063,7 @@
       </c>
       <c r="H372" s="11"/>
       <c r="I372" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="373" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -29730,7 +29730,7 @@
       </c>
       <c r="H413" s="11"/>
       <c r="I413" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="414" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -29757,7 +29757,7 @@
       </c>
       <c r="H414" s="11"/>
       <c r="I414" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="415" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -29944,7 +29944,7 @@
       </c>
       <c r="H425" s="11"/>
       <c r="I425" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="426" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -30527,7 +30527,7 @@
       </c>
       <c r="H461" s="11"/>
       <c r="I461" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="462" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -30870,11 +30870,11 @@
         <v>72</v>
       </c>
       <c r="G482" s="18" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
       <c r="H482" s="11"/>
       <c r="I482" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="483" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -31595,7 +31595,7 @@
       <c r="G527" s="18"/>
       <c r="H527" s="11"/>
       <c r="I527" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="528" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -31846,7 +31846,7 @@
       </c>
       <c r="H542" s="11"/>
       <c r="I542" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="543" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -31921,7 +31921,7 @@
       </c>
       <c r="H546" s="11"/>
       <c r="I546" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="547" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -32044,7 +32044,7 @@
       </c>
       <c r="H553" s="53"/>
       <c r="I553" s="11" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="554" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -32135,7 +32135,7 @@
       </c>
       <c r="H558" s="11"/>
       <c r="I558" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="559" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -32158,11 +32158,11 @@
         <v>1144</v>
       </c>
       <c r="G559" s="18" t="s">
-        <v>7345</v>
+        <v>7344</v>
       </c>
       <c r="H559" s="11"/>
       <c r="I559" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="560" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -32253,7 +32253,7 @@
       </c>
       <c r="H564" s="11"/>
       <c r="I564" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="565" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32280,7 +32280,7 @@
       </c>
       <c r="H565" s="11"/>
       <c r="I565" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="566" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32307,7 +32307,7 @@
       </c>
       <c r="H566" s="11"/>
       <c r="I566" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="567" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32334,7 +32334,7 @@
       </c>
       <c r="H567" s="11"/>
       <c r="I567" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="568" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -32361,7 +32361,7 @@
       </c>
       <c r="H568" s="11"/>
       <c r="I568" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="569" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -32388,7 +32388,7 @@
       </c>
       <c r="H569" s="11"/>
       <c r="I569" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="570" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -32415,7 +32415,7 @@
       </c>
       <c r="H570" s="11"/>
       <c r="I570" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="571" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32442,7 +32442,7 @@
       </c>
       <c r="H571" s="11"/>
       <c r="I571" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="572" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32469,7 +32469,7 @@
       </c>
       <c r="H572" s="11"/>
       <c r="I572" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="573" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32496,7 +32496,7 @@
       </c>
       <c r="H573" s="11"/>
       <c r="I573" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="574" spans="1:9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -32516,14 +32516,14 @@
         <v>1178</v>
       </c>
       <c r="F574" s="54" t="s">
-        <v>7347</v>
+        <v>7346</v>
       </c>
       <c r="G574" s="18" t="s">
         <v>7324</v>
       </c>
       <c r="H574" s="11"/>
       <c r="I574" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="575" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -32543,14 +32543,14 @@
         <v>1180</v>
       </c>
       <c r="F575" s="54" t="s">
-        <v>7346</v>
+        <v>7345</v>
       </c>
       <c r="G575" s="18" t="s">
         <v>7325</v>
       </c>
       <c r="H575" s="11"/>
       <c r="I575" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="576" spans="1:9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -32577,7 +32577,7 @@
       </c>
       <c r="H576" s="11"/>
       <c r="I576" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="577" spans="1:9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -32597,14 +32597,14 @@
         <v>1187</v>
       </c>
       <c r="F577" s="54" t="s">
-        <v>7348</v>
+        <v>7347</v>
       </c>
       <c r="G577" s="18" t="s">
         <v>7326</v>
       </c>
       <c r="H577" s="11"/>
       <c r="I577" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="578" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32631,7 +32631,7 @@
       </c>
       <c r="H578" s="11"/>
       <c r="I578" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="579" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32658,7 +32658,7 @@
       </c>
       <c r="H579" s="11"/>
       <c r="I579" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="580" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -32678,14 +32678,14 @@
         <v>1194</v>
       </c>
       <c r="F580" s="54" t="s">
-        <v>7349</v>
+        <v>7348</v>
       </c>
       <c r="G580" s="18" t="s">
         <v>7325</v>
       </c>
       <c r="H580" s="11"/>
       <c r="I580" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="581" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -32705,14 +32705,14 @@
         <v>1196</v>
       </c>
       <c r="F581" s="54" t="s">
-        <v>7350</v>
+        <v>7349</v>
       </c>
       <c r="G581" s="18" t="s">
         <v>7325</v>
       </c>
       <c r="H581" s="11"/>
       <c r="I581" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="582" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -32732,14 +32732,14 @@
         <v>1198</v>
       </c>
       <c r="F582" s="54" t="s">
-        <v>7351</v>
+        <v>7350</v>
       </c>
       <c r="G582" s="18" t="s">
         <v>7325</v>
       </c>
       <c r="H582" s="11"/>
       <c r="I582" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="583" spans="1:9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -32759,14 +32759,14 @@
         <v>1200</v>
       </c>
       <c r="F583" s="54" t="s">
-        <v>7352</v>
+        <v>7351</v>
       </c>
       <c r="G583" s="18" t="s">
         <v>7324</v>
       </c>
       <c r="H583" s="11"/>
       <c r="I583" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="584" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32793,7 +32793,7 @@
       </c>
       <c r="H584" s="11"/>
       <c r="I584" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="585" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -32820,7 +32820,7 @@
       </c>
       <c r="H585" s="11"/>
       <c r="I585" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="586" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -32847,7 +32847,7 @@
       </c>
       <c r="H586" s="11"/>
       <c r="I586" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="587" spans="1:9" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
@@ -32870,11 +32870,11 @@
         <v>1211</v>
       </c>
       <c r="G587" s="35" t="s">
-        <v>7357</v>
+        <v>7356</v>
       </c>
       <c r="H587" s="11"/>
       <c r="I587" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="588" spans="1:9" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -32897,11 +32897,11 @@
         <v>1214</v>
       </c>
       <c r="G588" s="35" t="s">
-        <v>7357</v>
+        <v>7356</v>
       </c>
       <c r="H588" s="11"/>
       <c r="I588" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="589" spans="1:9" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -32924,11 +32924,11 @@
         <v>1217</v>
       </c>
       <c r="G589" s="35" t="s">
-        <v>7357</v>
+        <v>7356</v>
       </c>
       <c r="H589" s="11"/>
       <c r="I589" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="590" spans="1:9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -32951,11 +32951,11 @@
         <v>1220</v>
       </c>
       <c r="G590" s="35" t="s">
-        <v>7357</v>
+        <v>7356</v>
       </c>
       <c r="H590" s="11"/>
       <c r="I590" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="591" spans="1:9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -32978,11 +32978,11 @@
         <v>1214</v>
       </c>
       <c r="G591" s="35" t="s">
-        <v>7357</v>
+        <v>7356</v>
       </c>
       <c r="H591" s="11"/>
       <c r="I591" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="592" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33009,10 +33009,10 @@
       </c>
       <c r="H592" s="11"/>
       <c r="I592" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="593" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="593" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A593" s="2" t="s">
         <v>1225</v>
       </c>
@@ -33028,10 +33028,10 @@
       <c r="G593" s="18"/>
       <c r="H593" s="11"/>
       <c r="I593" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="594" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="594" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A594" s="2" t="s">
         <v>1227</v>
       </c>
@@ -33047,10 +33047,10 @@
       <c r="G594" s="18"/>
       <c r="H594" s="11"/>
       <c r="I594" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="595" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="595" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A595" s="2" t="s">
         <v>1229</v>
       </c>
@@ -33066,10 +33066,10 @@
       <c r="G595" s="18"/>
       <c r="H595" s="11"/>
       <c r="I595" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="596" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="596" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A596" s="2" t="s">
         <v>1231</v>
       </c>
@@ -33085,10 +33085,10 @@
       <c r="G596" s="18"/>
       <c r="H596" s="11"/>
       <c r="I596" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="597" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="597" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A597" s="2" t="s">
         <v>1233</v>
       </c>
@@ -33104,10 +33104,10 @@
       <c r="G597" s="18"/>
       <c r="H597" s="11"/>
       <c r="I597" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="598" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="598" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A598" s="2" t="s">
         <v>1235</v>
       </c>
@@ -33123,7 +33123,7 @@
       <c r="G598" s="18"/>
       <c r="H598" s="11"/>
       <c r="I598" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="599" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -33150,10 +33150,10 @@
       </c>
       <c r="H599" s="11"/>
       <c r="I599" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="600" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="600" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A600" s="2" t="s">
         <v>1241</v>
       </c>
@@ -33169,10 +33169,10 @@
       <c r="G600" s="18"/>
       <c r="H600" s="11"/>
       <c r="I600" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="601" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="601" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A601" s="2" t="s">
         <v>1244</v>
       </c>
@@ -33188,10 +33188,10 @@
       <c r="G601" s="18"/>
       <c r="H601" s="11"/>
       <c r="I601" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="602" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="602" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A602" s="2" t="s">
         <v>1247</v>
       </c>
@@ -33207,10 +33207,10 @@
       <c r="G602" s="18"/>
       <c r="H602" s="11"/>
       <c r="I602" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="603" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="603" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A603" s="2" t="s">
         <v>1250</v>
       </c>
@@ -33226,10 +33226,10 @@
       <c r="G603" s="18"/>
       <c r="H603" s="11"/>
       <c r="I603" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="604" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="604" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A604" s="2" t="s">
         <v>1253</v>
       </c>
@@ -33245,10 +33245,10 @@
       <c r="G604" s="18"/>
       <c r="H604" s="11"/>
       <c r="I604" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="605" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="605" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A605" s="2" t="s">
         <v>1256</v>
       </c>
@@ -33264,10 +33264,10 @@
       <c r="G605" s="18"/>
       <c r="H605" s="11"/>
       <c r="I605" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="606" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="606" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A606" s="2" t="s">
         <v>1259</v>
       </c>
@@ -33283,10 +33283,10 @@
       <c r="G606" s="18"/>
       <c r="H606" s="11"/>
       <c r="I606" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="607" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="607" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A607" s="2" t="s">
         <v>1262</v>
       </c>
@@ -33302,10 +33302,10 @@
       <c r="G607" s="18"/>
       <c r="H607" s="11"/>
       <c r="I607" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="608" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="608" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A608" s="2" t="s">
         <v>1265</v>
       </c>
@@ -33321,10 +33321,10 @@
       <c r="G608" s="18"/>
       <c r="H608" s="11"/>
       <c r="I608" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="609" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="609" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A609" s="2" t="s">
         <v>1267</v>
       </c>
@@ -33340,10 +33340,10 @@
       <c r="G609" s="18"/>
       <c r="H609" s="11"/>
       <c r="I609" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="610" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="610" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A610" s="2" t="s">
         <v>1269</v>
       </c>
@@ -33359,10 +33359,10 @@
       <c r="G610" s="18"/>
       <c r="H610" s="11"/>
       <c r="I610" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="611" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="611" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A611" s="2" t="s">
         <v>1271</v>
       </c>
@@ -33378,10 +33378,10 @@
       <c r="G611" s="18"/>
       <c r="H611" s="11"/>
       <c r="I611" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="612" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="612" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A612" s="2" t="s">
         <v>1273</v>
       </c>
@@ -33397,10 +33397,10 @@
       <c r="G612" s="18"/>
       <c r="H612" s="11"/>
       <c r="I612" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="613" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="613" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A613" s="2" t="s">
         <v>1275</v>
       </c>
@@ -33416,10 +33416,10 @@
       <c r="G613" s="18"/>
       <c r="H613" s="11"/>
       <c r="I613" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="614" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="614" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A614" s="2" t="s">
         <v>1277</v>
       </c>
@@ -33435,10 +33435,10 @@
       <c r="G614" s="18"/>
       <c r="H614" s="11"/>
       <c r="I614" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="615" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="615" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A615" s="2" t="s">
         <v>1279</v>
       </c>
@@ -33454,10 +33454,10 @@
       <c r="G615" s="18"/>
       <c r="H615" s="11"/>
       <c r="I615" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="616" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="616" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A616" s="2" t="s">
         <v>1281</v>
       </c>
@@ -33473,10 +33473,10 @@
       <c r="G616" s="18"/>
       <c r="H616" s="11"/>
       <c r="I616" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="617" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="617" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A617" s="2" t="s">
         <v>1283</v>
       </c>
@@ -33492,10 +33492,10 @@
       <c r="G617" s="18"/>
       <c r="H617" s="11"/>
       <c r="I617" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="618" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="618" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A618" s="2" t="s">
         <v>1285</v>
       </c>
@@ -33511,10 +33511,10 @@
       <c r="G618" s="18"/>
       <c r="H618" s="11"/>
       <c r="I618" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="619" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="619" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A619" s="2" t="s">
         <v>1287</v>
       </c>
@@ -33530,10 +33530,10 @@
       <c r="G619" s="18"/>
       <c r="H619" s="11"/>
       <c r="I619" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="620" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="620" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A620" s="2" t="s">
         <v>1289</v>
       </c>
@@ -33549,7 +33549,7 @@
       <c r="G620" s="18"/>
       <c r="H620" s="11"/>
       <c r="I620" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="621" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33576,7 +33576,7 @@
       </c>
       <c r="H621" s="11"/>
       <c r="I621" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="622" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33603,10 +33603,10 @@
       </c>
       <c r="H622" s="11"/>
       <c r="I622" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="623" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="623" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A623" s="2" t="s">
         <v>1295</v>
       </c>
@@ -33622,10 +33622,10 @@
       <c r="G623" s="18"/>
       <c r="H623" s="11"/>
       <c r="I623" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="624" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="624" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A624" s="2" t="s">
         <v>1297</v>
       </c>
@@ -33641,10 +33641,10 @@
       <c r="G624" s="18"/>
       <c r="H624" s="11"/>
       <c r="I624" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="625" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="625" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A625" s="2" t="s">
         <v>1299</v>
       </c>
@@ -33660,10 +33660,10 @@
       <c r="G625" s="18"/>
       <c r="H625" s="11"/>
       <c r="I625" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="626" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="626" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A626" s="2" t="s">
         <v>1301</v>
       </c>
@@ -33679,10 +33679,10 @@
       <c r="G626" s="18"/>
       <c r="H626" s="11"/>
       <c r="I626" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="627" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="627" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A627" s="2" t="s">
         <v>1303</v>
       </c>
@@ -33698,10 +33698,10 @@
       <c r="G627" s="18"/>
       <c r="H627" s="11"/>
       <c r="I627" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="628" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="628" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A628" s="2" t="s">
         <v>1305</v>
       </c>
@@ -33717,10 +33717,10 @@
       <c r="G628" s="18"/>
       <c r="H628" s="11"/>
       <c r="I628" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="629" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="629" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A629" s="2" t="s">
         <v>1307</v>
       </c>
@@ -33736,7 +33736,7 @@
       <c r="G629" s="18"/>
       <c r="H629" s="11"/>
       <c r="I629" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="630" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -33763,7 +33763,7 @@
       </c>
       <c r="H630" s="11"/>
       <c r="I630" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="631" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -33790,10 +33790,10 @@
       </c>
       <c r="H631" s="11"/>
       <c r="I631" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="632" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="632" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A632" s="2" t="s">
         <v>1314</v>
       </c>
@@ -33809,10 +33809,10 @@
       <c r="G632" s="18"/>
       <c r="H632" s="11"/>
       <c r="I632" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="633" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="633" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A633" s="2" t="s">
         <v>1317</v>
       </c>
@@ -33828,10 +33828,10 @@
       <c r="G633" s="18"/>
       <c r="H633" s="11"/>
       <c r="I633" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="634" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="634" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A634" s="2" t="s">
         <v>1319</v>
       </c>
@@ -33847,10 +33847,10 @@
       <c r="G634" s="18"/>
       <c r="H634" s="11"/>
       <c r="I634" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="635" spans="1:9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="635" spans="1:9" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A635" s="2" t="s">
         <v>1322</v>
       </c>
@@ -33866,10 +33866,10 @@
       <c r="G635" s="18"/>
       <c r="H635" s="11"/>
       <c r="I635" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="636" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="636" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A636" s="2" t="s">
         <v>1325</v>
       </c>
@@ -33885,10 +33885,10 @@
       <c r="G636" s="18"/>
       <c r="H636" s="11"/>
       <c r="I636" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="637" spans="1:9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="637" spans="1:9" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A637" s="2" t="s">
         <v>1328</v>
       </c>
@@ -33904,10 +33904,10 @@
       <c r="G637" s="18"/>
       <c r="H637" s="11"/>
       <c r="I637" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="638" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="638" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A638" s="2" t="s">
         <v>1331</v>
       </c>
@@ -33923,10 +33923,10 @@
       <c r="G638" s="18"/>
       <c r="H638" s="11"/>
       <c r="I638" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="639" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="639" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A639" s="2" t="s">
         <v>1333</v>
       </c>
@@ -33942,10 +33942,10 @@
       <c r="G639" s="18"/>
       <c r="H639" s="11"/>
       <c r="I639" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="640" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="640" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A640" s="2" t="s">
         <v>1336</v>
       </c>
@@ -33961,10 +33961,10 @@
       <c r="G640" s="18"/>
       <c r="H640" s="11"/>
       <c r="I640" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="641" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="641" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A641" s="2" t="s">
         <v>1337</v>
       </c>
@@ -33980,10 +33980,10 @@
       <c r="G641" s="18"/>
       <c r="H641" s="11"/>
       <c r="I641" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="642" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="642" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A642" s="2" t="s">
         <v>1339</v>
       </c>
@@ -33999,10 +33999,10 @@
       <c r="G642" s="18"/>
       <c r="H642" s="11"/>
       <c r="I642" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="643" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="643" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A643" s="2" t="s">
         <v>1341</v>
       </c>
@@ -34018,10 +34018,10 @@
       <c r="G643" s="18"/>
       <c r="H643" s="11"/>
       <c r="I643" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="644" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="644" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A644" s="2" t="s">
         <v>1344</v>
       </c>
@@ -34037,7 +34037,7 @@
       <c r="G644" s="18"/>
       <c r="H644" s="11"/>
       <c r="I644" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="645" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -34064,10 +34064,10 @@
       </c>
       <c r="H645" s="11"/>
       <c r="I645" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="646" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="646" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A646" s="2" t="s">
         <v>1348</v>
       </c>
@@ -34083,10 +34083,10 @@
       <c r="G646" s="18"/>
       <c r="H646" s="11"/>
       <c r="I646" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="647" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="647" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A647" s="2" t="s">
         <v>1351</v>
       </c>
@@ -34102,10 +34102,10 @@
       <c r="G647" s="18"/>
       <c r="H647" s="11"/>
       <c r="I647" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="648" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="648" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A648" s="2" t="s">
         <v>1354</v>
       </c>
@@ -34121,10 +34121,10 @@
       <c r="G648" s="18"/>
       <c r="H648" s="11"/>
       <c r="I648" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="649" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="649" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A649" s="2" t="s">
         <v>1357</v>
       </c>
@@ -34140,10 +34140,10 @@
       <c r="G649" s="18"/>
       <c r="H649" s="11"/>
       <c r="I649" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="650" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="650" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A650" s="2" t="s">
         <v>1359</v>
       </c>
@@ -34159,10 +34159,10 @@
       <c r="G650" s="18"/>
       <c r="H650" s="11"/>
       <c r="I650" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="651" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="651" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A651" s="2" t="s">
         <v>1362</v>
       </c>
@@ -34178,10 +34178,10 @@
       <c r="G651" s="18"/>
       <c r="H651" s="11"/>
       <c r="I651" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="652" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="652" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A652" s="2" t="s">
         <v>1365</v>
       </c>
@@ -34197,7 +34197,7 @@
       <c r="G652" s="18"/>
       <c r="H652" s="11"/>
       <c r="I652" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="653" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -34224,10 +34224,10 @@
       </c>
       <c r="H653" s="11"/>
       <c r="I653" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="654" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="654" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A654" s="2" t="s">
         <v>1371</v>
       </c>
@@ -34243,10 +34243,10 @@
       <c r="G654" s="18"/>
       <c r="H654" s="11"/>
       <c r="I654" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="655" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="655" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A655" s="2" t="s">
         <v>1374</v>
       </c>
@@ -34262,10 +34262,10 @@
       <c r="G655" s="18"/>
       <c r="H655" s="11"/>
       <c r="I655" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="656" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="656" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A656" s="2" t="s">
         <v>1376</v>
       </c>
@@ -34281,10 +34281,10 @@
       <c r="G656" s="18"/>
       <c r="H656" s="11"/>
       <c r="I656" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="657" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="657" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A657" s="2" t="s">
         <v>1378</v>
       </c>
@@ -34300,10 +34300,10 @@
       <c r="G657" s="18"/>
       <c r="H657" s="11"/>
       <c r="I657" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="658" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="658" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A658" s="2" t="s">
         <v>1380</v>
       </c>
@@ -34319,7 +34319,7 @@
       <c r="G658" s="18"/>
       <c r="H658" s="11"/>
       <c r="I658" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="659" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -34346,10 +34346,10 @@
       </c>
       <c r="H659" s="11"/>
       <c r="I659" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="660" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="660" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A660" s="2" t="s">
         <v>1384</v>
       </c>
@@ -34365,10 +34365,10 @@
       <c r="G660" s="18"/>
       <c r="H660" s="11"/>
       <c r="I660" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="661" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="661" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A661" s="2" t="s">
         <v>1386</v>
       </c>
@@ -34384,10 +34384,10 @@
       <c r="G661" s="18"/>
       <c r="H661" s="11"/>
       <c r="I661" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="662" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="662" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A662" s="2" t="s">
         <v>1388</v>
       </c>
@@ -34403,10 +34403,10 @@
       <c r="G662" s="18"/>
       <c r="H662" s="11"/>
       <c r="I662" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="663" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="663" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A663" s="2" t="s">
         <v>1390</v>
       </c>
@@ -34422,10 +34422,10 @@
       <c r="G663" s="18"/>
       <c r="H663" s="11"/>
       <c r="I663" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="664" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="664" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A664" s="2" t="s">
         <v>1392</v>
       </c>
@@ -34441,10 +34441,10 @@
       <c r="G664" s="18"/>
       <c r="H664" s="11"/>
       <c r="I664" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="665" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="665" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A665" s="2" t="s">
         <v>1394</v>
       </c>
@@ -34460,10 +34460,10 @@
       <c r="G665" s="18"/>
       <c r="H665" s="11"/>
       <c r="I665" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="666" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="666" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A666" s="2" t="s">
         <v>1396</v>
       </c>
@@ -34479,10 +34479,10 @@
       <c r="G666" s="18"/>
       <c r="H666" s="11"/>
       <c r="I666" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="667" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="667" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A667" s="2" t="s">
         <v>1398</v>
       </c>
@@ -34498,10 +34498,10 @@
       <c r="G667" s="18"/>
       <c r="H667" s="11"/>
       <c r="I667" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="668" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="668" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A668" s="2" t="s">
         <v>1400</v>
       </c>
@@ -34517,10 +34517,10 @@
       <c r="G668" s="18"/>
       <c r="H668" s="11"/>
       <c r="I668" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="669" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="669" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A669" s="2" t="s">
         <v>1402</v>
       </c>
@@ -34536,10 +34536,10 @@
       <c r="G669" s="18"/>
       <c r="H669" s="11"/>
       <c r="I669" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="670" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="670" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A670" s="2" t="s">
         <v>1404</v>
       </c>
@@ -34555,10 +34555,10 @@
       <c r="G670" s="18"/>
       <c r="H670" s="11"/>
       <c r="I670" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="671" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="671" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A671" s="2" t="s">
         <v>1406</v>
       </c>
@@ -34574,10 +34574,10 @@
       <c r="G671" s="18"/>
       <c r="H671" s="11"/>
       <c r="I671" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="672" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="672" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A672" s="2" t="s">
         <v>1408</v>
       </c>
@@ -34593,10 +34593,10 @@
       <c r="G672" s="18"/>
       <c r="H672" s="11"/>
       <c r="I672" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="673" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="673" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A673" s="2" t="s">
         <v>1410</v>
       </c>
@@ -34612,10 +34612,10 @@
       <c r="G673" s="18"/>
       <c r="H673" s="11"/>
       <c r="I673" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="674" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="674" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A674" s="22" t="s">
         <v>1412</v>
       </c>
@@ -34656,15 +34656,15 @@
         <v>1417</v>
       </c>
       <c r="F675" s="55" t="s">
-        <v>7354</v>
+        <v>7353</v>
       </c>
       <c r="G675" s="18"/>
       <c r="H675" s="11"/>
       <c r="I675" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="676" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="676" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A676" s="2" t="s">
         <v>1419</v>
       </c>
@@ -34680,10 +34680,10 @@
       <c r="G676" s="18"/>
       <c r="H676" s="11"/>
       <c r="I676" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="677" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="677" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A677" s="2" t="s">
         <v>1422</v>
       </c>
@@ -34699,10 +34699,10 @@
       <c r="G677" s="18"/>
       <c r="H677" s="11"/>
       <c r="I677" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="678" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="678" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A678" s="2" t="s">
         <v>1424</v>
       </c>
@@ -34718,10 +34718,10 @@
       <c r="G678" s="18"/>
       <c r="H678" s="11"/>
       <c r="I678" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="679" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="679" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A679" s="2" t="s">
         <v>1427</v>
       </c>
@@ -34737,10 +34737,10 @@
       <c r="G679" s="18"/>
       <c r="H679" s="11"/>
       <c r="I679" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="680" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="680" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A680" s="2" t="s">
         <v>1429</v>
       </c>
@@ -34756,10 +34756,10 @@
       <c r="G680" s="18"/>
       <c r="H680" s="11"/>
       <c r="I680" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="681" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="681" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A681" s="2" t="s">
         <v>1432</v>
       </c>
@@ -34775,10 +34775,10 @@
       <c r="G681" s="18"/>
       <c r="H681" s="11"/>
       <c r="I681" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="682" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="682" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A682" s="2" t="s">
         <v>1435</v>
       </c>
@@ -34794,10 +34794,10 @@
       <c r="G682" s="18"/>
       <c r="H682" s="11"/>
       <c r="I682" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="683" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="683" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A683" s="2" t="s">
         <v>1438</v>
       </c>
@@ -34813,10 +34813,10 @@
       <c r="G683" s="18"/>
       <c r="H683" s="11"/>
       <c r="I683" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="684" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="684" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A684" s="2" t="s">
         <v>1441</v>
       </c>
@@ -34832,10 +34832,10 @@
       <c r="G684" s="18"/>
       <c r="H684" s="11"/>
       <c r="I684" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="685" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="685" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A685" s="2" t="s">
         <v>1443</v>
       </c>
@@ -34851,10 +34851,10 @@
       <c r="G685" s="18"/>
       <c r="H685" s="11"/>
       <c r="I685" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="686" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="686" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A686" s="2" t="s">
         <v>1446</v>
       </c>
@@ -34870,10 +34870,10 @@
       <c r="G686" s="18"/>
       <c r="H686" s="11"/>
       <c r="I686" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="687" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="687" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A687" s="2" t="s">
         <v>1449</v>
       </c>
@@ -34889,10 +34889,10 @@
       <c r="G687" s="18"/>
       <c r="H687" s="11"/>
       <c r="I687" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="688" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="688" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A688" s="2" t="s">
         <v>1451</v>
       </c>
@@ -34908,10 +34908,10 @@
       <c r="G688" s="18"/>
       <c r="H688" s="11"/>
       <c r="I688" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="689" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="689" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A689" s="2" t="s">
         <v>1454</v>
       </c>
@@ -34927,10 +34927,10 @@
       <c r="G689" s="18"/>
       <c r="H689" s="11"/>
       <c r="I689" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="690" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="690" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A690" s="2" t="s">
         <v>1456</v>
       </c>
@@ -34946,10 +34946,10 @@
       <c r="G690" s="18"/>
       <c r="H690" s="11"/>
       <c r="I690" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="691" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="691" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A691" s="2" t="s">
         <v>1458</v>
       </c>
@@ -34965,10 +34965,10 @@
       <c r="G691" s="18"/>
       <c r="H691" s="11"/>
       <c r="I691" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="692" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="692" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A692" s="2" t="s">
         <v>1461</v>
       </c>
@@ -34984,10 +34984,10 @@
       <c r="G692" s="18"/>
       <c r="H692" s="11"/>
       <c r="I692" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="693" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="693" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A693" s="2" t="s">
         <v>1463</v>
       </c>
@@ -35003,10 +35003,10 @@
       <c r="G693" s="18"/>
       <c r="H693" s="11"/>
       <c r="I693" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="694" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="694" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A694" s="2" t="s">
         <v>1465</v>
       </c>
@@ -35022,10 +35022,10 @@
       <c r="G694" s="18"/>
       <c r="H694" s="11"/>
       <c r="I694" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="695" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="695" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A695" s="2" t="s">
         <v>1467</v>
       </c>
@@ -35041,10 +35041,10 @@
       <c r="G695" s="18"/>
       <c r="H695" s="11"/>
       <c r="I695" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="696" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="696" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A696" s="2" t="s">
         <v>1469</v>
       </c>
@@ -35060,10 +35060,10 @@
       <c r="G696" s="18"/>
       <c r="H696" s="11"/>
       <c r="I696" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="697" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="697" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A697" s="2" t="s">
         <v>1472</v>
       </c>
@@ -35079,10 +35079,10 @@
       <c r="G697" s="18"/>
       <c r="H697" s="11"/>
       <c r="I697" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="698" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="698" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A698" s="2" t="s">
         <v>1475</v>
       </c>
@@ -35098,10 +35098,10 @@
       <c r="G698" s="18"/>
       <c r="H698" s="11"/>
       <c r="I698" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="699" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="699" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A699" s="2" t="s">
         <v>1478</v>
       </c>
@@ -35117,10 +35117,10 @@
       <c r="G699" s="18"/>
       <c r="H699" s="11"/>
       <c r="I699" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="700" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="700" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A700" s="2" t="s">
         <v>1481</v>
       </c>
@@ -35136,10 +35136,10 @@
       <c r="G700" s="18"/>
       <c r="H700" s="11"/>
       <c r="I700" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="701" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="701" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A701" s="2" t="s">
         <v>1484</v>
       </c>
@@ -35155,10 +35155,10 @@
       <c r="G701" s="18"/>
       <c r="H701" s="11"/>
       <c r="I701" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="702" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="702" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A702" s="2" t="s">
         <v>1487</v>
       </c>
@@ -35174,10 +35174,10 @@
       <c r="G702" s="18"/>
       <c r="H702" s="11"/>
       <c r="I702" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="703" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="703" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A703" s="2" t="s">
         <v>1490</v>
       </c>
@@ -35193,10 +35193,10 @@
       <c r="G703" s="18"/>
       <c r="H703" s="11"/>
       <c r="I703" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="704" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="704" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A704" s="2" t="s">
         <v>1493</v>
       </c>
@@ -35212,10 +35212,10 @@
       <c r="G704" s="18"/>
       <c r="H704" s="11"/>
       <c r="I704" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="705" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="705" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A705" s="2" t="s">
         <v>1496</v>
       </c>
@@ -35231,10 +35231,10 @@
       <c r="G705" s="18"/>
       <c r="H705" s="11"/>
       <c r="I705" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="706" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="706" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A706" s="2" t="s">
         <v>1499</v>
       </c>
@@ -35250,10 +35250,10 @@
       <c r="G706" s="18"/>
       <c r="H706" s="11"/>
       <c r="I706" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="707" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="707" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A707" s="2" t="s">
         <v>1502</v>
       </c>
@@ -35269,7 +35269,7 @@
       <c r="G707" s="18"/>
       <c r="H707" s="11"/>
       <c r="I707" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="708" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -35296,7 +35296,7 @@
       </c>
       <c r="H708" s="11"/>
       <c r="I708" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="709" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -35323,7 +35323,7 @@
       </c>
       <c r="H709" s="11"/>
       <c r="I709" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="710" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -35356,7 +35356,7 @@
       <c r="E711" s="27"/>
       <c r="F711" s="9"/>
       <c r="G711" s="35" t="s">
-        <v>7356</v>
+        <v>7355</v>
       </c>
       <c r="H711" s="11"/>
     </row>
@@ -35428,11 +35428,11 @@
         <v>1521</v>
       </c>
       <c r="G715" s="18" t="s">
-        <v>7355</v>
+        <v>7354</v>
       </c>
       <c r="H715" s="11"/>
       <c r="I715" s="11" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="716" spans="1:9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -35455,11 +35455,11 @@
         <v>1524</v>
       </c>
       <c r="G716" s="18" t="s">
-        <v>7333</v>
+        <v>7357</v>
       </c>
       <c r="H716" s="11"/>
       <c r="I716" s="11" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="717" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35482,12 +35482,10 @@
         <v>1172</v>
       </c>
       <c r="G717" s="18" t="s">
-        <v>7334</v>
+        <v>7333</v>
       </c>
       <c r="H717" s="11"/>
-      <c r="I717" s="11" t="s">
-        <v>7344</v>
-      </c>
+      <c r="I717" s="11"/>
     </row>
     <row r="718" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A718" s="40" t="s">
@@ -35509,12 +35507,10 @@
         <v>1158</v>
       </c>
       <c r="G718" s="18" t="s">
-        <v>7335</v>
+        <v>7334</v>
       </c>
       <c r="H718" s="11"/>
-      <c r="I718" s="11" t="s">
-        <v>7344</v>
-      </c>
+      <c r="I718" s="11"/>
     </row>
     <row r="719" spans="1:9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A719" s="40" t="s">
@@ -35536,11 +35532,11 @@
         <v>1536</v>
       </c>
       <c r="G719" s="18" t="s">
-        <v>7336</v>
+        <v>7335</v>
       </c>
       <c r="H719" s="11"/>
       <c r="I719" s="11" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="720" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -35557,11 +35553,11 @@
         <v>1539</v>
       </c>
       <c r="G720" s="18" t="s">
-        <v>7337</v>
+        <v>7336</v>
       </c>
       <c r="H720" s="53"/>
       <c r="I720" s="11" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="721" spans="1:10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -35578,11 +35574,11 @@
         <v>1542</v>
       </c>
       <c r="G721" s="18" t="s">
-        <v>7337</v>
+        <v>7336</v>
       </c>
       <c r="H721" s="53"/>
       <c r="I721" s="11" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="722" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
@@ -35599,11 +35595,11 @@
         <v>1545</v>
       </c>
       <c r="G722" s="18" t="s">
-        <v>7337</v>
+        <v>7336</v>
       </c>
       <c r="H722" s="53"/>
       <c r="I722" s="11" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="723" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
@@ -35620,11 +35616,11 @@
         <v>1158</v>
       </c>
       <c r="G723" s="18" t="s">
-        <v>7337</v>
+        <v>7336</v>
       </c>
       <c r="H723" s="53"/>
       <c r="I723" s="11" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="724" spans="1:10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -35647,14 +35643,14 @@
         <v>1115</v>
       </c>
       <c r="G724" s="18" t="s">
-        <v>7340</v>
+        <v>7339</v>
       </c>
       <c r="H724" s="11"/>
       <c r="I724" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
       <c r="J724" s="44" t="s">
-        <v>7339</v>
+        <v>7338</v>
       </c>
     </row>
     <row r="725" spans="1:10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35671,11 +35667,11 @@
         <v>1553</v>
       </c>
       <c r="G725" s="18" t="s">
-        <v>7337</v>
+        <v>7336</v>
       </c>
       <c r="H725" s="53"/>
       <c r="I725" s="11" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="726" spans="1:10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -35692,11 +35688,11 @@
         <v>1556</v>
       </c>
       <c r="G726" s="18" t="s">
-        <v>7337</v>
+        <v>7336</v>
       </c>
       <c r="H726" s="53"/>
       <c r="I726" s="11" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="727" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -35819,7 +35815,7 @@
       </c>
       <c r="H733" s="11"/>
       <c r="I733" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="734" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
@@ -35846,7 +35842,7 @@
       </c>
       <c r="H734" s="11"/>
       <c r="I734" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="735" spans="1:10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35873,7 +35869,7 @@
       </c>
       <c r="H735" s="11"/>
       <c r="I735" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="736" spans="1:10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35900,7 +35896,7 @@
       </c>
       <c r="H736" s="11"/>
       <c r="I736" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="737" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -35927,7 +35923,7 @@
       </c>
       <c r="H737" s="11"/>
       <c r="I737" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="738" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -35954,7 +35950,7 @@
       </c>
       <c r="H738" s="11"/>
       <c r="I738" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="739" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35981,7 +35977,7 @@
       </c>
       <c r="H739" s="11"/>
       <c r="I739" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="740" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -36008,7 +36004,7 @@
       </c>
       <c r="H740" s="11"/>
       <c r="I740" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="741" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -36035,7 +36031,7 @@
       </c>
       <c r="H741" s="11"/>
       <c r="I741" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="742" spans="1:9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -36062,7 +36058,7 @@
       </c>
       <c r="H742" s="11"/>
       <c r="I742" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="743" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -36089,7 +36085,7 @@
       </c>
       <c r="H743" s="11"/>
       <c r="I743" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="744" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -36898,7 +36894,7 @@
       </c>
       <c r="H793" s="11"/>
       <c r="I793" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="794" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -36925,7 +36921,7 @@
       </c>
       <c r="H794" s="11"/>
       <c r="I794" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="795" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -36952,7 +36948,7 @@
       </c>
       <c r="H795" s="11"/>
       <c r="I795" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="796" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -36979,7 +36975,7 @@
       </c>
       <c r="H796" s="11"/>
       <c r="I796" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="797" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -37006,7 +37002,7 @@
       </c>
       <c r="H797" s="11"/>
       <c r="I797" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="798" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -37033,7 +37029,7 @@
       </c>
       <c r="H798" s="11"/>
       <c r="I798" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="799" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -37156,7 +37152,7 @@
       </c>
       <c r="H805" s="11"/>
       <c r="I805" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="806" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -37525,11 +37521,11 @@
         <v>1310</v>
       </c>
       <c r="G828" s="18" t="s">
-        <v>7337</v>
+        <v>7336</v>
       </c>
       <c r="H828" s="53"/>
       <c r="I828" s="11" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="829" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -37546,11 +37542,11 @@
         <v>1539</v>
       </c>
       <c r="G829" s="18" t="s">
-        <v>7337</v>
+        <v>7336</v>
       </c>
       <c r="H829" s="53"/>
       <c r="I829" s="11" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="830" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -43461,11 +43457,11 @@
         <v>2322</v>
       </c>
       <c r="G1199" s="18" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
       <c r="H1199" s="11"/>
       <c r="I1199" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="1200" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -44896,7 +44892,7 @@
       </c>
       <c r="H1288" s="11"/>
       <c r="I1288" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="1289" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -46359,7 +46355,7 @@
       </c>
       <c r="H1379" s="11"/>
       <c r="I1379" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="1380" spans="1:9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -46376,11 +46372,11 @@
         <v>2851</v>
       </c>
       <c r="G1380" s="18" t="s">
-        <v>7337</v>
+        <v>7336</v>
       </c>
       <c r="H1380" s="53"/>
       <c r="I1380" s="11" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="1381" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -52215,7 +52211,7 @@
       </c>
       <c r="H1745" s="11"/>
       <c r="I1745" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="1746" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -52306,7 +52302,7 @@
       </c>
       <c r="H1750" s="11"/>
       <c r="I1750" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="1751" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -52985,11 +52981,11 @@
         <v>3672</v>
       </c>
       <c r="G1792" s="18" t="s">
-        <v>7353</v>
+        <v>7352</v>
       </c>
       <c r="H1792" s="11"/>
       <c r="I1792" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="1793" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -54084,7 +54080,7 @@
       </c>
       <c r="H1860" s="11"/>
       <c r="I1860" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="1861" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -54815,7 +54811,7 @@
       </c>
       <c r="H1905" s="11"/>
       <c r="I1905" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="1906" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -60806,7 +60802,7 @@
       </c>
       <c r="H2280" s="11"/>
       <c r="I2280" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="2281" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -63053,7 +63049,7 @@
       </c>
       <c r="H2420" s="11"/>
       <c r="I2420" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="2421" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -63784,7 +63780,7 @@
       </c>
       <c r="H2465" s="11"/>
       <c r="I2465" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
     <row r="2466" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -82229,24 +82225,23 @@
         <v>751</v>
       </c>
       <c r="G3621" s="52" t="s">
-        <v>7337</v>
+        <v>7336</v>
       </c>
       <c r="H3621" s="53"/>
       <c r="I3621" s="11" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:J3621">
     <filterColumn colId="0" showButton="0"/>
     <filterColumn colId="1" showButton="0"/>
-    <filterColumn colId="3" showButton="0"/>
-    <filterColumn colId="4" showButton="0"/>
-    <filterColumn colId="8">
+    <filterColumn colId="3" showButton="0">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
+    <filterColumn colId="4" showButton="0"/>
   </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>

</xml_diff>

<commit_message>
move "carbonyl oxidation to alkyne" to MOP properly
"carbonyl oxidation to alkyne" only declared in RXNO with an ID that was already taken in MOP --> copy all to MOP but mint new ID for it
</commit_message>
<xml_diff>
--- a/docs/#27_workfiles/MOP_vs_RXNO.xlsx
+++ b/docs/#27_workfiles/MOP_vs_RXNO.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11370" uniqueCount="7358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11371" uniqueCount="7358">
   <si>
     <t>ID</t>
   </si>
@@ -22084,9 +22084,6 @@
     <t>use MOP version, as its parent is more precise</t>
   </si>
   <si>
-    <t>"carbonyl oxidation to alkyne" has wrong ID, as this was taken by MOP already, thus needs a new ID to be minted in MOP</t>
-  </si>
-  <si>
     <t>"[3+2] cycloaddition" has wrong ID, as this was taken by MOP already, thus needs a new ID to be minted in MOP</t>
   </si>
   <si>
@@ -22172,6 +22169,9 @@
   </si>
   <si>
     <t>MOP:0000591 is the correct ID for 'carboxylation' --&gt; affects subclass RXNO:0000182; copy "has_participant some 'carboxy group'" axiom to MOP:0000591, also make comments to reflect this change; change parent (acylation) to be a subclass of  "organylation" as it is in RXNO and not just a sibling as it is in MOP right now</t>
+  </si>
+  <si>
+    <t>"carbonyl oxidation to alkyne" only declared in RXNO with an ID that was already taken in MOP --&gt; copy all to MOP but mint new ID for it</t>
   </si>
 </sst>
 </file>
@@ -23057,7 +23057,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A708" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G716" sqref="G716"/>
+      <selection pane="bottomLeft" activeCell="G717" sqref="G717"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23093,7 +23093,7 @@
         <v>7314</v>
       </c>
       <c r="I1" t="s">
-        <v>7337</v>
+        <v>7336</v>
       </c>
     </row>
     <row r="2" spans="1:9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -23186,11 +23186,11 @@
         <v>15</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="7" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -28561,7 +28561,7 @@
       </c>
       <c r="H342" s="11"/>
       <c r="I342" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="343" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -28972,7 +28972,7 @@
       </c>
       <c r="H367" s="11"/>
       <c r="I367" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="368" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -29063,7 +29063,7 @@
       </c>
       <c r="H372" s="11"/>
       <c r="I372" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="373" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -29730,7 +29730,7 @@
       </c>
       <c r="H413" s="11"/>
       <c r="I413" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="414" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -29757,7 +29757,7 @@
       </c>
       <c r="H414" s="11"/>
       <c r="I414" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="415" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -29944,7 +29944,7 @@
       </c>
       <c r="H425" s="11"/>
       <c r="I425" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="426" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -30527,7 +30527,7 @@
       </c>
       <c r="H461" s="11"/>
       <c r="I461" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="462" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -30870,11 +30870,11 @@
         <v>72</v>
       </c>
       <c r="G482" s="18" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
       <c r="H482" s="11"/>
       <c r="I482" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="483" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -31595,7 +31595,7 @@
       <c r="G527" s="18"/>
       <c r="H527" s="11"/>
       <c r="I527" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="528" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -31846,7 +31846,7 @@
       </c>
       <c r="H542" s="11"/>
       <c r="I542" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="543" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -31921,7 +31921,7 @@
       </c>
       <c r="H546" s="11"/>
       <c r="I546" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="547" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -32044,7 +32044,7 @@
       </c>
       <c r="H553" s="53"/>
       <c r="I553" s="11" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="554" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -32135,7 +32135,7 @@
       </c>
       <c r="H558" s="11"/>
       <c r="I558" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="559" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -32158,11 +32158,11 @@
         <v>1144</v>
       </c>
       <c r="G559" s="18" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
       <c r="H559" s="11"/>
       <c r="I559" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="560" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -32253,7 +32253,7 @@
       </c>
       <c r="H564" s="11"/>
       <c r="I564" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="565" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32280,7 +32280,7 @@
       </c>
       <c r="H565" s="11"/>
       <c r="I565" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="566" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32307,7 +32307,7 @@
       </c>
       <c r="H566" s="11"/>
       <c r="I566" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="567" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32334,7 +32334,7 @@
       </c>
       <c r="H567" s="11"/>
       <c r="I567" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="568" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -32361,7 +32361,7 @@
       </c>
       <c r="H568" s="11"/>
       <c r="I568" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="569" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -32388,7 +32388,7 @@
       </c>
       <c r="H569" s="11"/>
       <c r="I569" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="570" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -32415,7 +32415,7 @@
       </c>
       <c r="H570" s="11"/>
       <c r="I570" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="571" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32442,7 +32442,7 @@
       </c>
       <c r="H571" s="11"/>
       <c r="I571" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="572" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32469,7 +32469,7 @@
       </c>
       <c r="H572" s="11"/>
       <c r="I572" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="573" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32496,7 +32496,7 @@
       </c>
       <c r="H573" s="11"/>
       <c r="I573" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="574" spans="1:9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -32516,14 +32516,14 @@
         <v>1178</v>
       </c>
       <c r="F574" s="54" t="s">
-        <v>7346</v>
+        <v>7345</v>
       </c>
       <c r="G574" s="18" t="s">
         <v>7324</v>
       </c>
       <c r="H574" s="11"/>
       <c r="I574" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="575" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -32543,14 +32543,14 @@
         <v>1180</v>
       </c>
       <c r="F575" s="54" t="s">
-        <v>7345</v>
+        <v>7344</v>
       </c>
       <c r="G575" s="18" t="s">
         <v>7325</v>
       </c>
       <c r="H575" s="11"/>
       <c r="I575" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="576" spans="1:9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -32577,7 +32577,7 @@
       </c>
       <c r="H576" s="11"/>
       <c r="I576" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="577" spans="1:9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -32597,14 +32597,14 @@
         <v>1187</v>
       </c>
       <c r="F577" s="54" t="s">
-        <v>7347</v>
+        <v>7346</v>
       </c>
       <c r="G577" s="18" t="s">
         <v>7326</v>
       </c>
       <c r="H577" s="11"/>
       <c r="I577" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="578" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32631,7 +32631,7 @@
       </c>
       <c r="H578" s="11"/>
       <c r="I578" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="579" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32658,7 +32658,7 @@
       </c>
       <c r="H579" s="11"/>
       <c r="I579" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="580" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -32678,14 +32678,14 @@
         <v>1194</v>
       </c>
       <c r="F580" s="54" t="s">
-        <v>7348</v>
+        <v>7347</v>
       </c>
       <c r="G580" s="18" t="s">
         <v>7325</v>
       </c>
       <c r="H580" s="11"/>
       <c r="I580" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="581" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -32705,14 +32705,14 @@
         <v>1196</v>
       </c>
       <c r="F581" s="54" t="s">
-        <v>7349</v>
+        <v>7348</v>
       </c>
       <c r="G581" s="18" t="s">
         <v>7325</v>
       </c>
       <c r="H581" s="11"/>
       <c r="I581" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="582" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -32732,14 +32732,14 @@
         <v>1198</v>
       </c>
       <c r="F582" s="54" t="s">
-        <v>7350</v>
+        <v>7349</v>
       </c>
       <c r="G582" s="18" t="s">
         <v>7325</v>
       </c>
       <c r="H582" s="11"/>
       <c r="I582" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="583" spans="1:9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -32759,14 +32759,14 @@
         <v>1200</v>
       </c>
       <c r="F583" s="54" t="s">
-        <v>7351</v>
+        <v>7350</v>
       </c>
       <c r="G583" s="18" t="s">
         <v>7324</v>
       </c>
       <c r="H583" s="11"/>
       <c r="I583" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="584" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32793,7 +32793,7 @@
       </c>
       <c r="H584" s="11"/>
       <c r="I584" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="585" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -32820,7 +32820,7 @@
       </c>
       <c r="H585" s="11"/>
       <c r="I585" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="586" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -32847,7 +32847,7 @@
       </c>
       <c r="H586" s="11"/>
       <c r="I586" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="587" spans="1:9" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
@@ -32870,11 +32870,11 @@
         <v>1211</v>
       </c>
       <c r="G587" s="35" t="s">
-        <v>7356</v>
+        <v>7355</v>
       </c>
       <c r="H587" s="11"/>
       <c r="I587" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="588" spans="1:9" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -32897,11 +32897,11 @@
         <v>1214</v>
       </c>
       <c r="G588" s="35" t="s">
-        <v>7356</v>
+        <v>7355</v>
       </c>
       <c r="H588" s="11"/>
       <c r="I588" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="589" spans="1:9" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -32924,11 +32924,11 @@
         <v>1217</v>
       </c>
       <c r="G589" s="35" t="s">
-        <v>7356</v>
+        <v>7355</v>
       </c>
       <c r="H589" s="11"/>
       <c r="I589" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="590" spans="1:9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -32951,11 +32951,11 @@
         <v>1220</v>
       </c>
       <c r="G590" s="35" t="s">
-        <v>7356</v>
+        <v>7355</v>
       </c>
       <c r="H590" s="11"/>
       <c r="I590" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="591" spans="1:9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -32978,11 +32978,11 @@
         <v>1214</v>
       </c>
       <c r="G591" s="35" t="s">
-        <v>7356</v>
+        <v>7355</v>
       </c>
       <c r="H591" s="11"/>
       <c r="I591" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="592" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33009,7 +33009,7 @@
       </c>
       <c r="H592" s="11"/>
       <c r="I592" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="593" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33028,7 +33028,7 @@
       <c r="G593" s="18"/>
       <c r="H593" s="11"/>
       <c r="I593" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="594" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33047,7 +33047,7 @@
       <c r="G594" s="18"/>
       <c r="H594" s="11"/>
       <c r="I594" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="595" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33066,7 +33066,7 @@
       <c r="G595" s="18"/>
       <c r="H595" s="11"/>
       <c r="I595" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="596" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33085,7 +33085,7 @@
       <c r="G596" s="18"/>
       <c r="H596" s="11"/>
       <c r="I596" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="597" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33104,7 +33104,7 @@
       <c r="G597" s="18"/>
       <c r="H597" s="11"/>
       <c r="I597" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="598" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33123,7 +33123,7 @@
       <c r="G598" s="18"/>
       <c r="H598" s="11"/>
       <c r="I598" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="599" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -33150,7 +33150,7 @@
       </c>
       <c r="H599" s="11"/>
       <c r="I599" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="600" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -33169,7 +33169,7 @@
       <c r="G600" s="18"/>
       <c r="H600" s="11"/>
       <c r="I600" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="601" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -33188,7 +33188,7 @@
       <c r="G601" s="18"/>
       <c r="H601" s="11"/>
       <c r="I601" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="602" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -33207,7 +33207,7 @@
       <c r="G602" s="18"/>
       <c r="H602" s="11"/>
       <c r="I602" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="603" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -33226,7 +33226,7 @@
       <c r="G603" s="18"/>
       <c r="H603" s="11"/>
       <c r="I603" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="604" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -33245,7 +33245,7 @@
       <c r="G604" s="18"/>
       <c r="H604" s="11"/>
       <c r="I604" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="605" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -33264,7 +33264,7 @@
       <c r="G605" s="18"/>
       <c r="H605" s="11"/>
       <c r="I605" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="606" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -33283,7 +33283,7 @@
       <c r="G606" s="18"/>
       <c r="H606" s="11"/>
       <c r="I606" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="607" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33302,7 +33302,7 @@
       <c r="G607" s="18"/>
       <c r="H607" s="11"/>
       <c r="I607" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="608" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33321,7 +33321,7 @@
       <c r="G608" s="18"/>
       <c r="H608" s="11"/>
       <c r="I608" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="609" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33340,7 +33340,7 @@
       <c r="G609" s="18"/>
       <c r="H609" s="11"/>
       <c r="I609" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="610" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33359,7 +33359,7 @@
       <c r="G610" s="18"/>
       <c r="H610" s="11"/>
       <c r="I610" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="611" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33378,7 +33378,7 @@
       <c r="G611" s="18"/>
       <c r="H611" s="11"/>
       <c r="I611" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="612" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33397,7 +33397,7 @@
       <c r="G612" s="18"/>
       <c r="H612" s="11"/>
       <c r="I612" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="613" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33416,7 +33416,7 @@
       <c r="G613" s="18"/>
       <c r="H613" s="11"/>
       <c r="I613" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="614" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33435,7 +33435,7 @@
       <c r="G614" s="18"/>
       <c r="H614" s="11"/>
       <c r="I614" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="615" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33454,7 +33454,7 @@
       <c r="G615" s="18"/>
       <c r="H615" s="11"/>
       <c r="I615" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="616" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -33473,7 +33473,7 @@
       <c r="G616" s="18"/>
       <c r="H616" s="11"/>
       <c r="I616" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="617" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33492,7 +33492,7 @@
       <c r="G617" s="18"/>
       <c r="H617" s="11"/>
       <c r="I617" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="618" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33511,7 +33511,7 @@
       <c r="G618" s="18"/>
       <c r="H618" s="11"/>
       <c r="I618" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="619" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -33530,7 +33530,7 @@
       <c r="G619" s="18"/>
       <c r="H619" s="11"/>
       <c r="I619" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="620" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -33549,7 +33549,7 @@
       <c r="G620" s="18"/>
       <c r="H620" s="11"/>
       <c r="I620" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="621" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33576,7 +33576,7 @@
       </c>
       <c r="H621" s="11"/>
       <c r="I621" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="622" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33603,7 +33603,7 @@
       </c>
       <c r="H622" s="11"/>
       <c r="I622" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="623" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33622,7 +33622,7 @@
       <c r="G623" s="18"/>
       <c r="H623" s="11"/>
       <c r="I623" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="624" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33641,7 +33641,7 @@
       <c r="G624" s="18"/>
       <c r="H624" s="11"/>
       <c r="I624" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="625" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33660,7 +33660,7 @@
       <c r="G625" s="18"/>
       <c r="H625" s="11"/>
       <c r="I625" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="626" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33679,7 +33679,7 @@
       <c r="G626" s="18"/>
       <c r="H626" s="11"/>
       <c r="I626" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="627" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33698,7 +33698,7 @@
       <c r="G627" s="18"/>
       <c r="H627" s="11"/>
       <c r="I627" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="628" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33717,7 +33717,7 @@
       <c r="G628" s="18"/>
       <c r="H628" s="11"/>
       <c r="I628" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="629" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33736,7 +33736,7 @@
       <c r="G629" s="18"/>
       <c r="H629" s="11"/>
       <c r="I629" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="630" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -33763,7 +33763,7 @@
       </c>
       <c r="H630" s="11"/>
       <c r="I630" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="631" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -33790,7 +33790,7 @@
       </c>
       <c r="H631" s="11"/>
       <c r="I631" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="632" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -33809,7 +33809,7 @@
       <c r="G632" s="18"/>
       <c r="H632" s="11"/>
       <c r="I632" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="633" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33828,7 +33828,7 @@
       <c r="G633" s="18"/>
       <c r="H633" s="11"/>
       <c r="I633" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="634" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -33847,7 +33847,7 @@
       <c r="G634" s="18"/>
       <c r="H634" s="11"/>
       <c r="I634" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="635" spans="1:9" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -33866,7 +33866,7 @@
       <c r="G635" s="18"/>
       <c r="H635" s="11"/>
       <c r="I635" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="636" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -33885,7 +33885,7 @@
       <c r="G636" s="18"/>
       <c r="H636" s="11"/>
       <c r="I636" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="637" spans="1:9" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -33904,7 +33904,7 @@
       <c r="G637" s="18"/>
       <c r="H637" s="11"/>
       <c r="I637" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="638" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33923,7 +33923,7 @@
       <c r="G638" s="18"/>
       <c r="H638" s="11"/>
       <c r="I638" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="639" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -33942,7 +33942,7 @@
       <c r="G639" s="18"/>
       <c r="H639" s="11"/>
       <c r="I639" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="640" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33961,7 +33961,7 @@
       <c r="G640" s="18"/>
       <c r="H640" s="11"/>
       <c r="I640" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="641" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -33980,7 +33980,7 @@
       <c r="G641" s="18"/>
       <c r="H641" s="11"/>
       <c r="I641" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="642" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -33999,7 +33999,7 @@
       <c r="G642" s="18"/>
       <c r="H642" s="11"/>
       <c r="I642" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="643" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -34018,7 +34018,7 @@
       <c r="G643" s="18"/>
       <c r="H643" s="11"/>
       <c r="I643" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="644" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -34037,7 +34037,7 @@
       <c r="G644" s="18"/>
       <c r="H644" s="11"/>
       <c r="I644" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="645" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -34064,7 +34064,7 @@
       </c>
       <c r="H645" s="11"/>
       <c r="I645" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="646" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -34083,7 +34083,7 @@
       <c r="G646" s="18"/>
       <c r="H646" s="11"/>
       <c r="I646" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="647" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -34102,7 +34102,7 @@
       <c r="G647" s="18"/>
       <c r="H647" s="11"/>
       <c r="I647" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="648" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -34121,7 +34121,7 @@
       <c r="G648" s="18"/>
       <c r="H648" s="11"/>
       <c r="I648" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="649" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34140,7 +34140,7 @@
       <c r="G649" s="18"/>
       <c r="H649" s="11"/>
       <c r="I649" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="650" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -34159,7 +34159,7 @@
       <c r="G650" s="18"/>
       <c r="H650" s="11"/>
       <c r="I650" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="651" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -34178,7 +34178,7 @@
       <c r="G651" s="18"/>
       <c r="H651" s="11"/>
       <c r="I651" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="652" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -34197,7 +34197,7 @@
       <c r="G652" s="18"/>
       <c r="H652" s="11"/>
       <c r="I652" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="653" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -34224,7 +34224,7 @@
       </c>
       <c r="H653" s="11"/>
       <c r="I653" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="654" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -34243,7 +34243,7 @@
       <c r="G654" s="18"/>
       <c r="H654" s="11"/>
       <c r="I654" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="655" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34262,7 +34262,7 @@
       <c r="G655" s="18"/>
       <c r="H655" s="11"/>
       <c r="I655" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="656" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34281,7 +34281,7 @@
       <c r="G656" s="18"/>
       <c r="H656" s="11"/>
       <c r="I656" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="657" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34300,7 +34300,7 @@
       <c r="G657" s="18"/>
       <c r="H657" s="11"/>
       <c r="I657" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="658" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34319,7 +34319,7 @@
       <c r="G658" s="18"/>
       <c r="H658" s="11"/>
       <c r="I658" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="659" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -34346,7 +34346,7 @@
       </c>
       <c r="H659" s="11"/>
       <c r="I659" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="660" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -34365,7 +34365,7 @@
       <c r="G660" s="18"/>
       <c r="H660" s="11"/>
       <c r="I660" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="661" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -34384,7 +34384,7 @@
       <c r="G661" s="18"/>
       <c r="H661" s="11"/>
       <c r="I661" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="662" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -34403,7 +34403,7 @@
       <c r="G662" s="18"/>
       <c r="H662" s="11"/>
       <c r="I662" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="663" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -34422,7 +34422,7 @@
       <c r="G663" s="18"/>
       <c r="H663" s="11"/>
       <c r="I663" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="664" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -34441,7 +34441,7 @@
       <c r="G664" s="18"/>
       <c r="H664" s="11"/>
       <c r="I664" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="665" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -34460,7 +34460,7 @@
       <c r="G665" s="18"/>
       <c r="H665" s="11"/>
       <c r="I665" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="666" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -34479,7 +34479,7 @@
       <c r="G666" s="18"/>
       <c r="H666" s="11"/>
       <c r="I666" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="667" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34498,7 +34498,7 @@
       <c r="G667" s="18"/>
       <c r="H667" s="11"/>
       <c r="I667" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="668" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34517,7 +34517,7 @@
       <c r="G668" s="18"/>
       <c r="H668" s="11"/>
       <c r="I668" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="669" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34536,7 +34536,7 @@
       <c r="G669" s="18"/>
       <c r="H669" s="11"/>
       <c r="I669" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="670" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34555,7 +34555,7 @@
       <c r="G670" s="18"/>
       <c r="H670" s="11"/>
       <c r="I670" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="671" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34574,7 +34574,7 @@
       <c r="G671" s="18"/>
       <c r="H671" s="11"/>
       <c r="I671" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="672" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34593,7 +34593,7 @@
       <c r="G672" s="18"/>
       <c r="H672" s="11"/>
       <c r="I672" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="673" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34612,7 +34612,7 @@
       <c r="G673" s="18"/>
       <c r="H673" s="11"/>
       <c r="I673" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="674" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -34656,12 +34656,12 @@
         <v>1417</v>
       </c>
       <c r="F675" s="55" t="s">
-        <v>7353</v>
+        <v>7352</v>
       </c>
       <c r="G675" s="18"/>
       <c r="H675" s="11"/>
       <c r="I675" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="676" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -34680,7 +34680,7 @@
       <c r="G676" s="18"/>
       <c r="H676" s="11"/>
       <c r="I676" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="677" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34699,7 +34699,7 @@
       <c r="G677" s="18"/>
       <c r="H677" s="11"/>
       <c r="I677" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="678" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34718,7 +34718,7 @@
       <c r="G678" s="18"/>
       <c r="H678" s="11"/>
       <c r="I678" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="679" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34737,7 +34737,7 @@
       <c r="G679" s="18"/>
       <c r="H679" s="11"/>
       <c r="I679" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="680" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -34756,7 +34756,7 @@
       <c r="G680" s="18"/>
       <c r="H680" s="11"/>
       <c r="I680" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="681" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -34775,7 +34775,7 @@
       <c r="G681" s="18"/>
       <c r="H681" s="11"/>
       <c r="I681" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="682" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -34794,7 +34794,7 @@
       <c r="G682" s="18"/>
       <c r="H682" s="11"/>
       <c r="I682" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="683" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -34813,7 +34813,7 @@
       <c r="G683" s="18"/>
       <c r="H683" s="11"/>
       <c r="I683" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="684" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34832,7 +34832,7 @@
       <c r="G684" s="18"/>
       <c r="H684" s="11"/>
       <c r="I684" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="685" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -34851,7 +34851,7 @@
       <c r="G685" s="18"/>
       <c r="H685" s="11"/>
       <c r="I685" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="686" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -34870,7 +34870,7 @@
       <c r="G686" s="18"/>
       <c r="H686" s="11"/>
       <c r="I686" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="687" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -34889,7 +34889,7 @@
       <c r="G687" s="18"/>
       <c r="H687" s="11"/>
       <c r="I687" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="688" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -34908,7 +34908,7 @@
       <c r="G688" s="18"/>
       <c r="H688" s="11"/>
       <c r="I688" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="689" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -34927,7 +34927,7 @@
       <c r="G689" s="18"/>
       <c r="H689" s="11"/>
       <c r="I689" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="690" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34946,7 +34946,7 @@
       <c r="G690" s="18"/>
       <c r="H690" s="11"/>
       <c r="I690" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="691" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -34965,7 +34965,7 @@
       <c r="G691" s="18"/>
       <c r="H691" s="11"/>
       <c r="I691" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="692" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -34984,7 +34984,7 @@
       <c r="G692" s="18"/>
       <c r="H692" s="11"/>
       <c r="I692" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="693" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -35003,7 +35003,7 @@
       <c r="G693" s="18"/>
       <c r="H693" s="11"/>
       <c r="I693" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="694" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -35022,7 +35022,7 @@
       <c r="G694" s="18"/>
       <c r="H694" s="11"/>
       <c r="I694" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="695" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -35041,7 +35041,7 @@
       <c r="G695" s="18"/>
       <c r="H695" s="11"/>
       <c r="I695" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="696" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -35060,7 +35060,7 @@
       <c r="G696" s="18"/>
       <c r="H696" s="11"/>
       <c r="I696" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="697" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -35079,7 +35079,7 @@
       <c r="G697" s="18"/>
       <c r="H697" s="11"/>
       <c r="I697" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="698" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -35098,7 +35098,7 @@
       <c r="G698" s="18"/>
       <c r="H698" s="11"/>
       <c r="I698" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="699" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -35117,7 +35117,7 @@
       <c r="G699" s="18"/>
       <c r="H699" s="11"/>
       <c r="I699" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="700" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -35136,7 +35136,7 @@
       <c r="G700" s="18"/>
       <c r="H700" s="11"/>
       <c r="I700" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="701" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -35155,7 +35155,7 @@
       <c r="G701" s="18"/>
       <c r="H701" s="11"/>
       <c r="I701" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="702" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -35174,7 +35174,7 @@
       <c r="G702" s="18"/>
       <c r="H702" s="11"/>
       <c r="I702" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="703" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -35193,7 +35193,7 @@
       <c r="G703" s="18"/>
       <c r="H703" s="11"/>
       <c r="I703" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="704" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -35212,7 +35212,7 @@
       <c r="G704" s="18"/>
       <c r="H704" s="11"/>
       <c r="I704" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="705" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -35231,7 +35231,7 @@
       <c r="G705" s="18"/>
       <c r="H705" s="11"/>
       <c r="I705" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="706" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -35250,7 +35250,7 @@
       <c r="G706" s="18"/>
       <c r="H706" s="11"/>
       <c r="I706" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="707" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -35269,7 +35269,7 @@
       <c r="G707" s="18"/>
       <c r="H707" s="11"/>
       <c r="I707" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="708" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -35296,7 +35296,7 @@
       </c>
       <c r="H708" s="11"/>
       <c r="I708" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="709" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -35323,7 +35323,7 @@
       </c>
       <c r="H709" s="11"/>
       <c r="I709" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="710" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -35356,7 +35356,7 @@
       <c r="E711" s="27"/>
       <c r="F711" s="9"/>
       <c r="G711" s="35" t="s">
-        <v>7355</v>
+        <v>7354</v>
       </c>
       <c r="H711" s="11"/>
     </row>
@@ -35428,11 +35428,11 @@
         <v>1521</v>
       </c>
       <c r="G715" s="18" t="s">
-        <v>7354</v>
+        <v>7353</v>
       </c>
       <c r="H715" s="11"/>
       <c r="I715" s="11" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="716" spans="1:9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -35455,11 +35455,11 @@
         <v>1524</v>
       </c>
       <c r="G716" s="18" t="s">
-        <v>7357</v>
+        <v>7356</v>
       </c>
       <c r="H716" s="11"/>
       <c r="I716" s="11" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="717" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35482,10 +35482,12 @@
         <v>1172</v>
       </c>
       <c r="G717" s="18" t="s">
-        <v>7333</v>
+        <v>7357</v>
       </c>
       <c r="H717" s="11"/>
-      <c r="I717" s="11"/>
+      <c r="I717" s="11" t="s">
+        <v>7342</v>
+      </c>
     </row>
     <row r="718" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A718" s="40" t="s">
@@ -35507,7 +35509,7 @@
         <v>1158</v>
       </c>
       <c r="G718" s="18" t="s">
-        <v>7334</v>
+        <v>7333</v>
       </c>
       <c r="H718" s="11"/>
       <c r="I718" s="11"/>
@@ -35532,11 +35534,11 @@
         <v>1536</v>
       </c>
       <c r="G719" s="18" t="s">
-        <v>7335</v>
+        <v>7334</v>
       </c>
       <c r="H719" s="11"/>
       <c r="I719" s="11" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="720" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -35553,11 +35555,11 @@
         <v>1539</v>
       </c>
       <c r="G720" s="18" t="s">
-        <v>7336</v>
+        <v>7335</v>
       </c>
       <c r="H720" s="53"/>
       <c r="I720" s="11" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="721" spans="1:10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -35574,11 +35576,11 @@
         <v>1542</v>
       </c>
       <c r="G721" s="18" t="s">
-        <v>7336</v>
+        <v>7335</v>
       </c>
       <c r="H721" s="53"/>
       <c r="I721" s="11" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="722" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
@@ -35595,11 +35597,11 @@
         <v>1545</v>
       </c>
       <c r="G722" s="18" t="s">
-        <v>7336</v>
+        <v>7335</v>
       </c>
       <c r="H722" s="53"/>
       <c r="I722" s="11" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="723" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
@@ -35616,11 +35618,11 @@
         <v>1158</v>
       </c>
       <c r="G723" s="18" t="s">
-        <v>7336</v>
+        <v>7335</v>
       </c>
       <c r="H723" s="53"/>
       <c r="I723" s="11" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="724" spans="1:10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -35643,14 +35645,14 @@
         <v>1115</v>
       </c>
       <c r="G724" s="18" t="s">
-        <v>7339</v>
+        <v>7338</v>
       </c>
       <c r="H724" s="11"/>
       <c r="I724" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
       <c r="J724" s="44" t="s">
-        <v>7338</v>
+        <v>7337</v>
       </c>
     </row>
     <row r="725" spans="1:10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35667,11 +35669,11 @@
         <v>1553</v>
       </c>
       <c r="G725" s="18" t="s">
-        <v>7336</v>
+        <v>7335</v>
       </c>
       <c r="H725" s="53"/>
       <c r="I725" s="11" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="726" spans="1:10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -35688,11 +35690,11 @@
         <v>1556</v>
       </c>
       <c r="G726" s="18" t="s">
-        <v>7336</v>
+        <v>7335</v>
       </c>
       <c r="H726" s="53"/>
       <c r="I726" s="11" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="727" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -35815,7 +35817,7 @@
       </c>
       <c r="H733" s="11"/>
       <c r="I733" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="734" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
@@ -35842,7 +35844,7 @@
       </c>
       <c r="H734" s="11"/>
       <c r="I734" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="735" spans="1:10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35869,7 +35871,7 @@
       </c>
       <c r="H735" s="11"/>
       <c r="I735" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="736" spans="1:10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35896,7 +35898,7 @@
       </c>
       <c r="H736" s="11"/>
       <c r="I736" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="737" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -35923,7 +35925,7 @@
       </c>
       <c r="H737" s="11"/>
       <c r="I737" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="738" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -35950,7 +35952,7 @@
       </c>
       <c r="H738" s="11"/>
       <c r="I738" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="739" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35977,7 +35979,7 @@
       </c>
       <c r="H739" s="11"/>
       <c r="I739" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="740" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -36004,7 +36006,7 @@
       </c>
       <c r="H740" s="11"/>
       <c r="I740" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="741" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -36031,7 +36033,7 @@
       </c>
       <c r="H741" s="11"/>
       <c r="I741" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="742" spans="1:9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -36058,7 +36060,7 @@
       </c>
       <c r="H742" s="11"/>
       <c r="I742" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="743" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -36085,7 +36087,7 @@
       </c>
       <c r="H743" s="11"/>
       <c r="I743" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="744" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -36894,7 +36896,7 @@
       </c>
       <c r="H793" s="11"/>
       <c r="I793" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="794" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -36921,7 +36923,7 @@
       </c>
       <c r="H794" s="11"/>
       <c r="I794" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="795" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -36948,7 +36950,7 @@
       </c>
       <c r="H795" s="11"/>
       <c r="I795" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="796" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -36975,7 +36977,7 @@
       </c>
       <c r="H796" s="11"/>
       <c r="I796" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="797" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -37002,7 +37004,7 @@
       </c>
       <c r="H797" s="11"/>
       <c r="I797" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="798" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -37029,7 +37031,7 @@
       </c>
       <c r="H798" s="11"/>
       <c r="I798" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="799" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -37152,7 +37154,7 @@
       </c>
       <c r="H805" s="11"/>
       <c r="I805" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="806" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -37521,11 +37523,11 @@
         <v>1310</v>
       </c>
       <c r="G828" s="18" t="s">
-        <v>7336</v>
+        <v>7335</v>
       </c>
       <c r="H828" s="53"/>
       <c r="I828" s="11" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="829" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -37542,11 +37544,11 @@
         <v>1539</v>
       </c>
       <c r="G829" s="18" t="s">
-        <v>7336</v>
+        <v>7335</v>
       </c>
       <c r="H829" s="53"/>
       <c r="I829" s="11" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="830" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -43457,11 +43459,11 @@
         <v>2322</v>
       </c>
       <c r="G1199" s="18" t="s">
-        <v>7340</v>
+        <v>7339</v>
       </c>
       <c r="H1199" s="11"/>
       <c r="I1199" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="1200" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -44892,7 +44894,7 @@
       </c>
       <c r="H1288" s="11"/>
       <c r="I1288" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="1289" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -46355,7 +46357,7 @@
       </c>
       <c r="H1379" s="11"/>
       <c r="I1379" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="1380" spans="1:9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -46372,11 +46374,11 @@
         <v>2851</v>
       </c>
       <c r="G1380" s="18" t="s">
-        <v>7336</v>
+        <v>7335</v>
       </c>
       <c r="H1380" s="53"/>
       <c r="I1380" s="11" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="1381" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -52211,7 +52213,7 @@
       </c>
       <c r="H1745" s="11"/>
       <c r="I1745" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="1746" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -52302,7 +52304,7 @@
       </c>
       <c r="H1750" s="11"/>
       <c r="I1750" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="1751" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -52981,11 +52983,11 @@
         <v>3672</v>
       </c>
       <c r="G1792" s="18" t="s">
-        <v>7352</v>
+        <v>7351</v>
       </c>
       <c r="H1792" s="11"/>
       <c r="I1792" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="1793" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -54080,7 +54082,7 @@
       </c>
       <c r="H1860" s="11"/>
       <c r="I1860" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="1861" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -54811,7 +54813,7 @@
       </c>
       <c r="H1905" s="11"/>
       <c r="I1905" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="1906" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -60802,7 +60804,7 @@
       </c>
       <c r="H2280" s="11"/>
       <c r="I2280" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="2281" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -63049,7 +63051,7 @@
       </c>
       <c r="H2420" s="11"/>
       <c r="I2420" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="2421" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -63780,7 +63782,7 @@
       </c>
       <c r="H2465" s="11"/>
       <c r="I2465" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="2466" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -82225,11 +82227,11 @@
         <v>751</v>
       </c>
       <c r="G3621" s="52" t="s">
-        <v>7336</v>
+        <v>7335</v>
       </c>
       <c r="H3621" s="53"/>
       <c r="I3621" s="11" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move "[3+2] cycloaddition" to MOP
"[3+2] cycloaddition" had wrong ID in RXNO, was taken by MOP already, thus needed a new ID to be minted in MOP
</commit_message>
<xml_diff>
--- a/docs/#27_workfiles/MOP_vs_RXNO.xlsx
+++ b/docs/#27_workfiles/MOP_vs_RXNO.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11371" uniqueCount="7358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11372" uniqueCount="7358">
   <si>
     <t>ID</t>
   </si>
@@ -22084,9 +22084,6 @@
     <t>use MOP version, as its parent is more precise</t>
   </si>
   <si>
-    <t>"[3+2] cycloaddition" has wrong ID, as this was taken by MOP already, thus needs a new ID to be minted in MOP</t>
-  </si>
-  <si>
     <t>"enolization" is MOP:0000672 --&gt; wrong ID in RXNO; sync axioms and use MOP parent 'keto-enol tautomerisation'</t>
   </si>
   <si>
@@ -22172,6 +22169,9 @@
   </si>
   <si>
     <t>"carbonyl oxidation to alkyne" only declared in RXNO with an ID that was already taken in MOP --&gt; copy all to MOP but mint new ID for it</t>
+  </si>
+  <si>
+    <t>"[3+2] cycloaddition" had wrong ID in RXNO, was taken by MOP already, thus needed a new ID to be minted in MOP</t>
   </si>
 </sst>
 </file>
@@ -23057,7 +23057,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A708" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G717" sqref="G717"/>
+      <selection pane="bottomLeft" activeCell="G719" sqref="G719"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23093,7 +23093,7 @@
         <v>7314</v>
       </c>
       <c r="I1" t="s">
-        <v>7336</v>
+        <v>7335</v>
       </c>
     </row>
     <row r="2" spans="1:9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -23186,11 +23186,11 @@
         <v>15</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="7" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -28561,7 +28561,7 @@
       </c>
       <c r="H342" s="11"/>
       <c r="I342" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="343" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -28972,7 +28972,7 @@
       </c>
       <c r="H367" s="11"/>
       <c r="I367" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="368" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -29063,7 +29063,7 @@
       </c>
       <c r="H372" s="11"/>
       <c r="I372" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="373" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -29730,7 +29730,7 @@
       </c>
       <c r="H413" s="11"/>
       <c r="I413" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="414" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -29757,7 +29757,7 @@
       </c>
       <c r="H414" s="11"/>
       <c r="I414" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="415" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -29944,7 +29944,7 @@
       </c>
       <c r="H425" s="11"/>
       <c r="I425" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="426" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -30527,7 +30527,7 @@
       </c>
       <c r="H461" s="11"/>
       <c r="I461" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="462" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -30870,11 +30870,11 @@
         <v>72</v>
       </c>
       <c r="G482" s="18" t="s">
-        <v>7340</v>
+        <v>7339</v>
       </c>
       <c r="H482" s="11"/>
       <c r="I482" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="483" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -31595,7 +31595,7 @@
       <c r="G527" s="18"/>
       <c r="H527" s="11"/>
       <c r="I527" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="528" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -31846,7 +31846,7 @@
       </c>
       <c r="H542" s="11"/>
       <c r="I542" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="543" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -31921,7 +31921,7 @@
       </c>
       <c r="H546" s="11"/>
       <c r="I546" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="547" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -32044,7 +32044,7 @@
       </c>
       <c r="H553" s="53"/>
       <c r="I553" s="11" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="554" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -32135,7 +32135,7 @@
       </c>
       <c r="H558" s="11"/>
       <c r="I558" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="559" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -32158,11 +32158,11 @@
         <v>1144</v>
       </c>
       <c r="G559" s="18" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
       <c r="H559" s="11"/>
       <c r="I559" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="560" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -32253,7 +32253,7 @@
       </c>
       <c r="H564" s="11"/>
       <c r="I564" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="565" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32280,7 +32280,7 @@
       </c>
       <c r="H565" s="11"/>
       <c r="I565" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="566" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32307,7 +32307,7 @@
       </c>
       <c r="H566" s="11"/>
       <c r="I566" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="567" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32334,7 +32334,7 @@
       </c>
       <c r="H567" s="11"/>
       <c r="I567" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="568" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -32361,7 +32361,7 @@
       </c>
       <c r="H568" s="11"/>
       <c r="I568" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="569" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -32388,7 +32388,7 @@
       </c>
       <c r="H569" s="11"/>
       <c r="I569" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="570" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -32415,7 +32415,7 @@
       </c>
       <c r="H570" s="11"/>
       <c r="I570" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="571" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32442,7 +32442,7 @@
       </c>
       <c r="H571" s="11"/>
       <c r="I571" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="572" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32469,7 +32469,7 @@
       </c>
       <c r="H572" s="11"/>
       <c r="I572" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="573" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32496,7 +32496,7 @@
       </c>
       <c r="H573" s="11"/>
       <c r="I573" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="574" spans="1:9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -32516,14 +32516,14 @@
         <v>1178</v>
       </c>
       <c r="F574" s="54" t="s">
-        <v>7345</v>
+        <v>7344</v>
       </c>
       <c r="G574" s="18" t="s">
         <v>7324</v>
       </c>
       <c r="H574" s="11"/>
       <c r="I574" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="575" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -32543,14 +32543,14 @@
         <v>1180</v>
       </c>
       <c r="F575" s="54" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
       <c r="G575" s="18" t="s">
         <v>7325</v>
       </c>
       <c r="H575" s="11"/>
       <c r="I575" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="576" spans="1:9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -32577,7 +32577,7 @@
       </c>
       <c r="H576" s="11"/>
       <c r="I576" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="577" spans="1:9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -32597,14 +32597,14 @@
         <v>1187</v>
       </c>
       <c r="F577" s="54" t="s">
-        <v>7346</v>
+        <v>7345</v>
       </c>
       <c r="G577" s="18" t="s">
         <v>7326</v>
       </c>
       <c r="H577" s="11"/>
       <c r="I577" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="578" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32631,7 +32631,7 @@
       </c>
       <c r="H578" s="11"/>
       <c r="I578" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="579" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32658,7 +32658,7 @@
       </c>
       <c r="H579" s="11"/>
       <c r="I579" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="580" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -32678,14 +32678,14 @@
         <v>1194</v>
       </c>
       <c r="F580" s="54" t="s">
-        <v>7347</v>
+        <v>7346</v>
       </c>
       <c r="G580" s="18" t="s">
         <v>7325</v>
       </c>
       <c r="H580" s="11"/>
       <c r="I580" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="581" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -32705,14 +32705,14 @@
         <v>1196</v>
       </c>
       <c r="F581" s="54" t="s">
-        <v>7348</v>
+        <v>7347</v>
       </c>
       <c r="G581" s="18" t="s">
         <v>7325</v>
       </c>
       <c r="H581" s="11"/>
       <c r="I581" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="582" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -32732,14 +32732,14 @@
         <v>1198</v>
       </c>
       <c r="F582" s="54" t="s">
-        <v>7349</v>
+        <v>7348</v>
       </c>
       <c r="G582" s="18" t="s">
         <v>7325</v>
       </c>
       <c r="H582" s="11"/>
       <c r="I582" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="583" spans="1:9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -32759,14 +32759,14 @@
         <v>1200</v>
       </c>
       <c r="F583" s="54" t="s">
-        <v>7350</v>
+        <v>7349</v>
       </c>
       <c r="G583" s="18" t="s">
         <v>7324</v>
       </c>
       <c r="H583" s="11"/>
       <c r="I583" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="584" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32793,7 +32793,7 @@
       </c>
       <c r="H584" s="11"/>
       <c r="I584" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="585" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -32820,7 +32820,7 @@
       </c>
       <c r="H585" s="11"/>
       <c r="I585" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="586" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -32847,7 +32847,7 @@
       </c>
       <c r="H586" s="11"/>
       <c r="I586" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="587" spans="1:9" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
@@ -32870,11 +32870,11 @@
         <v>1211</v>
       </c>
       <c r="G587" s="35" t="s">
-        <v>7355</v>
+        <v>7354</v>
       </c>
       <c r="H587" s="11"/>
       <c r="I587" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="588" spans="1:9" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -32897,11 +32897,11 @@
         <v>1214</v>
       </c>
       <c r="G588" s="35" t="s">
-        <v>7355</v>
+        <v>7354</v>
       </c>
       <c r="H588" s="11"/>
       <c r="I588" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="589" spans="1:9" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -32924,11 +32924,11 @@
         <v>1217</v>
       </c>
       <c r="G589" s="35" t="s">
-        <v>7355</v>
+        <v>7354</v>
       </c>
       <c r="H589" s="11"/>
       <c r="I589" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="590" spans="1:9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -32951,11 +32951,11 @@
         <v>1220</v>
       </c>
       <c r="G590" s="35" t="s">
-        <v>7355</v>
+        <v>7354</v>
       </c>
       <c r="H590" s="11"/>
       <c r="I590" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="591" spans="1:9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -32978,11 +32978,11 @@
         <v>1214</v>
       </c>
       <c r="G591" s="35" t="s">
-        <v>7355</v>
+        <v>7354</v>
       </c>
       <c r="H591" s="11"/>
       <c r="I591" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="592" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33009,7 +33009,7 @@
       </c>
       <c r="H592" s="11"/>
       <c r="I592" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="593" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33028,7 +33028,7 @@
       <c r="G593" s="18"/>
       <c r="H593" s="11"/>
       <c r="I593" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="594" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33047,7 +33047,7 @@
       <c r="G594" s="18"/>
       <c r="H594" s="11"/>
       <c r="I594" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="595" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33066,7 +33066,7 @@
       <c r="G595" s="18"/>
       <c r="H595" s="11"/>
       <c r="I595" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="596" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33085,7 +33085,7 @@
       <c r="G596" s="18"/>
       <c r="H596" s="11"/>
       <c r="I596" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="597" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33104,7 +33104,7 @@
       <c r="G597" s="18"/>
       <c r="H597" s="11"/>
       <c r="I597" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="598" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33123,7 +33123,7 @@
       <c r="G598" s="18"/>
       <c r="H598" s="11"/>
       <c r="I598" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="599" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -33150,7 +33150,7 @@
       </c>
       <c r="H599" s="11"/>
       <c r="I599" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="600" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -33169,7 +33169,7 @@
       <c r="G600" s="18"/>
       <c r="H600" s="11"/>
       <c r="I600" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="601" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -33188,7 +33188,7 @@
       <c r="G601" s="18"/>
       <c r="H601" s="11"/>
       <c r="I601" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="602" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -33207,7 +33207,7 @@
       <c r="G602" s="18"/>
       <c r="H602" s="11"/>
       <c r="I602" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="603" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -33226,7 +33226,7 @@
       <c r="G603" s="18"/>
       <c r="H603" s="11"/>
       <c r="I603" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="604" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -33245,7 +33245,7 @@
       <c r="G604" s="18"/>
       <c r="H604" s="11"/>
       <c r="I604" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="605" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -33264,7 +33264,7 @@
       <c r="G605" s="18"/>
       <c r="H605" s="11"/>
       <c r="I605" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="606" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -33283,7 +33283,7 @@
       <c r="G606" s="18"/>
       <c r="H606" s="11"/>
       <c r="I606" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="607" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33302,7 +33302,7 @@
       <c r="G607" s="18"/>
       <c r="H607" s="11"/>
       <c r="I607" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="608" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33321,7 +33321,7 @@
       <c r="G608" s="18"/>
       <c r="H608" s="11"/>
       <c r="I608" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="609" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33340,7 +33340,7 @@
       <c r="G609" s="18"/>
       <c r="H609" s="11"/>
       <c r="I609" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="610" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33359,7 +33359,7 @@
       <c r="G610" s="18"/>
       <c r="H610" s="11"/>
       <c r="I610" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="611" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33378,7 +33378,7 @@
       <c r="G611" s="18"/>
       <c r="H611" s="11"/>
       <c r="I611" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="612" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33397,7 +33397,7 @@
       <c r="G612" s="18"/>
       <c r="H612" s="11"/>
       <c r="I612" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="613" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33416,7 +33416,7 @@
       <c r="G613" s="18"/>
       <c r="H613" s="11"/>
       <c r="I613" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="614" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33435,7 +33435,7 @@
       <c r="G614" s="18"/>
       <c r="H614" s="11"/>
       <c r="I614" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="615" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33454,7 +33454,7 @@
       <c r="G615" s="18"/>
       <c r="H615" s="11"/>
       <c r="I615" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="616" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -33473,7 +33473,7 @@
       <c r="G616" s="18"/>
       <c r="H616" s="11"/>
       <c r="I616" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="617" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33492,7 +33492,7 @@
       <c r="G617" s="18"/>
       <c r="H617" s="11"/>
       <c r="I617" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="618" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33511,7 +33511,7 @@
       <c r="G618" s="18"/>
       <c r="H618" s="11"/>
       <c r="I618" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="619" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -33530,7 +33530,7 @@
       <c r="G619" s="18"/>
       <c r="H619" s="11"/>
       <c r="I619" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="620" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -33549,7 +33549,7 @@
       <c r="G620" s="18"/>
       <c r="H620" s="11"/>
       <c r="I620" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="621" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33576,7 +33576,7 @@
       </c>
       <c r="H621" s="11"/>
       <c r="I621" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="622" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33603,7 +33603,7 @@
       </c>
       <c r="H622" s="11"/>
       <c r="I622" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="623" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33622,7 +33622,7 @@
       <c r="G623" s="18"/>
       <c r="H623" s="11"/>
       <c r="I623" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="624" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33641,7 +33641,7 @@
       <c r="G624" s="18"/>
       <c r="H624" s="11"/>
       <c r="I624" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="625" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33660,7 +33660,7 @@
       <c r="G625" s="18"/>
       <c r="H625" s="11"/>
       <c r="I625" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="626" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33679,7 +33679,7 @@
       <c r="G626" s="18"/>
       <c r="H626" s="11"/>
       <c r="I626" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="627" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33698,7 +33698,7 @@
       <c r="G627" s="18"/>
       <c r="H627" s="11"/>
       <c r="I627" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="628" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33717,7 +33717,7 @@
       <c r="G628" s="18"/>
       <c r="H628" s="11"/>
       <c r="I628" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="629" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33736,7 +33736,7 @@
       <c r="G629" s="18"/>
       <c r="H629" s="11"/>
       <c r="I629" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="630" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -33763,7 +33763,7 @@
       </c>
       <c r="H630" s="11"/>
       <c r="I630" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="631" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -33790,7 +33790,7 @@
       </c>
       <c r="H631" s="11"/>
       <c r="I631" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="632" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -33809,7 +33809,7 @@
       <c r="G632" s="18"/>
       <c r="H632" s="11"/>
       <c r="I632" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="633" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33828,7 +33828,7 @@
       <c r="G633" s="18"/>
       <c r="H633" s="11"/>
       <c r="I633" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="634" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -33847,7 +33847,7 @@
       <c r="G634" s="18"/>
       <c r="H634" s="11"/>
       <c r="I634" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="635" spans="1:9" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -33866,7 +33866,7 @@
       <c r="G635" s="18"/>
       <c r="H635" s="11"/>
       <c r="I635" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="636" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -33885,7 +33885,7 @@
       <c r="G636" s="18"/>
       <c r="H636" s="11"/>
       <c r="I636" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="637" spans="1:9" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -33904,7 +33904,7 @@
       <c r="G637" s="18"/>
       <c r="H637" s="11"/>
       <c r="I637" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="638" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33923,7 +33923,7 @@
       <c r="G638" s="18"/>
       <c r="H638" s="11"/>
       <c r="I638" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="639" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -33942,7 +33942,7 @@
       <c r="G639" s="18"/>
       <c r="H639" s="11"/>
       <c r="I639" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="640" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -33961,7 +33961,7 @@
       <c r="G640" s="18"/>
       <c r="H640" s="11"/>
       <c r="I640" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="641" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -33980,7 +33980,7 @@
       <c r="G641" s="18"/>
       <c r="H641" s="11"/>
       <c r="I641" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="642" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -33999,7 +33999,7 @@
       <c r="G642" s="18"/>
       <c r="H642" s="11"/>
       <c r="I642" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="643" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -34018,7 +34018,7 @@
       <c r="G643" s="18"/>
       <c r="H643" s="11"/>
       <c r="I643" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="644" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -34037,7 +34037,7 @@
       <c r="G644" s="18"/>
       <c r="H644" s="11"/>
       <c r="I644" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="645" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -34064,7 +34064,7 @@
       </c>
       <c r="H645" s="11"/>
       <c r="I645" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="646" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -34083,7 +34083,7 @@
       <c r="G646" s="18"/>
       <c r="H646" s="11"/>
       <c r="I646" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="647" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -34102,7 +34102,7 @@
       <c r="G647" s="18"/>
       <c r="H647" s="11"/>
       <c r="I647" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="648" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -34121,7 +34121,7 @@
       <c r="G648" s="18"/>
       <c r="H648" s="11"/>
       <c r="I648" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="649" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34140,7 +34140,7 @@
       <c r="G649" s="18"/>
       <c r="H649" s="11"/>
       <c r="I649" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="650" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -34159,7 +34159,7 @@
       <c r="G650" s="18"/>
       <c r="H650" s="11"/>
       <c r="I650" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="651" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -34178,7 +34178,7 @@
       <c r="G651" s="18"/>
       <c r="H651" s="11"/>
       <c r="I651" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="652" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -34197,7 +34197,7 @@
       <c r="G652" s="18"/>
       <c r="H652" s="11"/>
       <c r="I652" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="653" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -34224,7 +34224,7 @@
       </c>
       <c r="H653" s="11"/>
       <c r="I653" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="654" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -34243,7 +34243,7 @@
       <c r="G654" s="18"/>
       <c r="H654" s="11"/>
       <c r="I654" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="655" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34262,7 +34262,7 @@
       <c r="G655" s="18"/>
       <c r="H655" s="11"/>
       <c r="I655" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="656" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34281,7 +34281,7 @@
       <c r="G656" s="18"/>
       <c r="H656" s="11"/>
       <c r="I656" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="657" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34300,7 +34300,7 @@
       <c r="G657" s="18"/>
       <c r="H657" s="11"/>
       <c r="I657" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="658" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34319,7 +34319,7 @@
       <c r="G658" s="18"/>
       <c r="H658" s="11"/>
       <c r="I658" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="659" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -34346,7 +34346,7 @@
       </c>
       <c r="H659" s="11"/>
       <c r="I659" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="660" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -34365,7 +34365,7 @@
       <c r="G660" s="18"/>
       <c r="H660" s="11"/>
       <c r="I660" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="661" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -34384,7 +34384,7 @@
       <c r="G661" s="18"/>
       <c r="H661" s="11"/>
       <c r="I661" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="662" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -34403,7 +34403,7 @@
       <c r="G662" s="18"/>
       <c r="H662" s="11"/>
       <c r="I662" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="663" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -34422,7 +34422,7 @@
       <c r="G663" s="18"/>
       <c r="H663" s="11"/>
       <c r="I663" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="664" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -34441,7 +34441,7 @@
       <c r="G664" s="18"/>
       <c r="H664" s="11"/>
       <c r="I664" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="665" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -34460,7 +34460,7 @@
       <c r="G665" s="18"/>
       <c r="H665" s="11"/>
       <c r="I665" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="666" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -34479,7 +34479,7 @@
       <c r="G666" s="18"/>
       <c r="H666" s="11"/>
       <c r="I666" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="667" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34498,7 +34498,7 @@
       <c r="G667" s="18"/>
       <c r="H667" s="11"/>
       <c r="I667" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="668" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34517,7 +34517,7 @@
       <c r="G668" s="18"/>
       <c r="H668" s="11"/>
       <c r="I668" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="669" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34536,7 +34536,7 @@
       <c r="G669" s="18"/>
       <c r="H669" s="11"/>
       <c r="I669" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="670" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34555,7 +34555,7 @@
       <c r="G670" s="18"/>
       <c r="H670" s="11"/>
       <c r="I670" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="671" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34574,7 +34574,7 @@
       <c r="G671" s="18"/>
       <c r="H671" s="11"/>
       <c r="I671" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="672" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34593,7 +34593,7 @@
       <c r="G672" s="18"/>
       <c r="H672" s="11"/>
       <c r="I672" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="673" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34612,7 +34612,7 @@
       <c r="G673" s="18"/>
       <c r="H673" s="11"/>
       <c r="I673" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="674" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -34656,12 +34656,12 @@
         <v>1417</v>
       </c>
       <c r="F675" s="55" t="s">
-        <v>7352</v>
+        <v>7351</v>
       </c>
       <c r="G675" s="18"/>
       <c r="H675" s="11"/>
       <c r="I675" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="676" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -34680,7 +34680,7 @@
       <c r="G676" s="18"/>
       <c r="H676" s="11"/>
       <c r="I676" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="677" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34699,7 +34699,7 @@
       <c r="G677" s="18"/>
       <c r="H677" s="11"/>
       <c r="I677" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="678" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34718,7 +34718,7 @@
       <c r="G678" s="18"/>
       <c r="H678" s="11"/>
       <c r="I678" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="679" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34737,7 +34737,7 @@
       <c r="G679" s="18"/>
       <c r="H679" s="11"/>
       <c r="I679" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="680" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -34756,7 +34756,7 @@
       <c r="G680" s="18"/>
       <c r="H680" s="11"/>
       <c r="I680" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="681" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -34775,7 +34775,7 @@
       <c r="G681" s="18"/>
       <c r="H681" s="11"/>
       <c r="I681" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="682" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -34794,7 +34794,7 @@
       <c r="G682" s="18"/>
       <c r="H682" s="11"/>
       <c r="I682" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="683" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -34813,7 +34813,7 @@
       <c r="G683" s="18"/>
       <c r="H683" s="11"/>
       <c r="I683" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="684" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34832,7 +34832,7 @@
       <c r="G684" s="18"/>
       <c r="H684" s="11"/>
       <c r="I684" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="685" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -34851,7 +34851,7 @@
       <c r="G685" s="18"/>
       <c r="H685" s="11"/>
       <c r="I685" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="686" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -34870,7 +34870,7 @@
       <c r="G686" s="18"/>
       <c r="H686" s="11"/>
       <c r="I686" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="687" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -34889,7 +34889,7 @@
       <c r="G687" s="18"/>
       <c r="H687" s="11"/>
       <c r="I687" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="688" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -34908,7 +34908,7 @@
       <c r="G688" s="18"/>
       <c r="H688" s="11"/>
       <c r="I688" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="689" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -34927,7 +34927,7 @@
       <c r="G689" s="18"/>
       <c r="H689" s="11"/>
       <c r="I689" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="690" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -34946,7 +34946,7 @@
       <c r="G690" s="18"/>
       <c r="H690" s="11"/>
       <c r="I690" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="691" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -34965,7 +34965,7 @@
       <c r="G691" s="18"/>
       <c r="H691" s="11"/>
       <c r="I691" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="692" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -34984,7 +34984,7 @@
       <c r="G692" s="18"/>
       <c r="H692" s="11"/>
       <c r="I692" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="693" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -35003,7 +35003,7 @@
       <c r="G693" s="18"/>
       <c r="H693" s="11"/>
       <c r="I693" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="694" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -35022,7 +35022,7 @@
       <c r="G694" s="18"/>
       <c r="H694" s="11"/>
       <c r="I694" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="695" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -35041,7 +35041,7 @@
       <c r="G695" s="18"/>
       <c r="H695" s="11"/>
       <c r="I695" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="696" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -35060,7 +35060,7 @@
       <c r="G696" s="18"/>
       <c r="H696" s="11"/>
       <c r="I696" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="697" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -35079,7 +35079,7 @@
       <c r="G697" s="18"/>
       <c r="H697" s="11"/>
       <c r="I697" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="698" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -35098,7 +35098,7 @@
       <c r="G698" s="18"/>
       <c r="H698" s="11"/>
       <c r="I698" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="699" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -35117,7 +35117,7 @@
       <c r="G699" s="18"/>
       <c r="H699" s="11"/>
       <c r="I699" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="700" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -35136,7 +35136,7 @@
       <c r="G700" s="18"/>
       <c r="H700" s="11"/>
       <c r="I700" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="701" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -35155,7 +35155,7 @@
       <c r="G701" s="18"/>
       <c r="H701" s="11"/>
       <c r="I701" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="702" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -35174,7 +35174,7 @@
       <c r="G702" s="18"/>
       <c r="H702" s="11"/>
       <c r="I702" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="703" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -35193,7 +35193,7 @@
       <c r="G703" s="18"/>
       <c r="H703" s="11"/>
       <c r="I703" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="704" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -35212,7 +35212,7 @@
       <c r="G704" s="18"/>
       <c r="H704" s="11"/>
       <c r="I704" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="705" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -35231,7 +35231,7 @@
       <c r="G705" s="18"/>
       <c r="H705" s="11"/>
       <c r="I705" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="706" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -35250,7 +35250,7 @@
       <c r="G706" s="18"/>
       <c r="H706" s="11"/>
       <c r="I706" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="707" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -35269,7 +35269,7 @@
       <c r="G707" s="18"/>
       <c r="H707" s="11"/>
       <c r="I707" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="708" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -35296,7 +35296,7 @@
       </c>
       <c r="H708" s="11"/>
       <c r="I708" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="709" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -35323,7 +35323,7 @@
       </c>
       <c r="H709" s="11"/>
       <c r="I709" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="710" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -35356,7 +35356,7 @@
       <c r="E711" s="27"/>
       <c r="F711" s="9"/>
       <c r="G711" s="35" t="s">
-        <v>7354</v>
+        <v>7353</v>
       </c>
       <c r="H711" s="11"/>
     </row>
@@ -35428,11 +35428,11 @@
         <v>1521</v>
       </c>
       <c r="G715" s="18" t="s">
-        <v>7353</v>
+        <v>7352</v>
       </c>
       <c r="H715" s="11"/>
       <c r="I715" s="11" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="716" spans="1:9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -35455,11 +35455,11 @@
         <v>1524</v>
       </c>
       <c r="G716" s="18" t="s">
-        <v>7356</v>
+        <v>7355</v>
       </c>
       <c r="H716" s="11"/>
       <c r="I716" s="11" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="717" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35482,11 +35482,11 @@
         <v>1172</v>
       </c>
       <c r="G717" s="18" t="s">
-        <v>7357</v>
+        <v>7356</v>
       </c>
       <c r="H717" s="11"/>
       <c r="I717" s="11" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="718" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -35509,10 +35509,12 @@
         <v>1158</v>
       </c>
       <c r="G718" s="18" t="s">
-        <v>7333</v>
+        <v>7357</v>
       </c>
       <c r="H718" s="11"/>
-      <c r="I718" s="11"/>
+      <c r="I718" s="11" t="s">
+        <v>7341</v>
+      </c>
     </row>
     <row r="719" spans="1:9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A719" s="40" t="s">
@@ -35534,11 +35536,11 @@
         <v>1536</v>
       </c>
       <c r="G719" s="18" t="s">
-        <v>7334</v>
+        <v>7333</v>
       </c>
       <c r="H719" s="11"/>
       <c r="I719" s="11" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="720" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -35555,11 +35557,11 @@
         <v>1539</v>
       </c>
       <c r="G720" s="18" t="s">
-        <v>7335</v>
+        <v>7334</v>
       </c>
       <c r="H720" s="53"/>
       <c r="I720" s="11" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="721" spans="1:10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -35576,11 +35578,11 @@
         <v>1542</v>
       </c>
       <c r="G721" s="18" t="s">
-        <v>7335</v>
+        <v>7334</v>
       </c>
       <c r="H721" s="53"/>
       <c r="I721" s="11" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="722" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
@@ -35597,11 +35599,11 @@
         <v>1545</v>
       </c>
       <c r="G722" s="18" t="s">
-        <v>7335</v>
+        <v>7334</v>
       </c>
       <c r="H722" s="53"/>
       <c r="I722" s="11" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="723" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
@@ -35618,11 +35620,11 @@
         <v>1158</v>
       </c>
       <c r="G723" s="18" t="s">
-        <v>7335</v>
+        <v>7334</v>
       </c>
       <c r="H723" s="53"/>
       <c r="I723" s="11" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="724" spans="1:10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -35645,14 +35647,14 @@
         <v>1115</v>
       </c>
       <c r="G724" s="18" t="s">
-        <v>7338</v>
+        <v>7337</v>
       </c>
       <c r="H724" s="11"/>
       <c r="I724" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
       <c r="J724" s="44" t="s">
-        <v>7337</v>
+        <v>7336</v>
       </c>
     </row>
     <row r="725" spans="1:10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35669,11 +35671,11 @@
         <v>1553</v>
       </c>
       <c r="G725" s="18" t="s">
-        <v>7335</v>
+        <v>7334</v>
       </c>
       <c r="H725" s="53"/>
       <c r="I725" s="11" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="726" spans="1:10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -35690,11 +35692,11 @@
         <v>1556</v>
       </c>
       <c r="G726" s="18" t="s">
-        <v>7335</v>
+        <v>7334</v>
       </c>
       <c r="H726" s="53"/>
       <c r="I726" s="11" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="727" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -35817,7 +35819,7 @@
       </c>
       <c r="H733" s="11"/>
       <c r="I733" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="734" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
@@ -35844,7 +35846,7 @@
       </c>
       <c r="H734" s="11"/>
       <c r="I734" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="735" spans="1:10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35871,7 +35873,7 @@
       </c>
       <c r="H735" s="11"/>
       <c r="I735" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="736" spans="1:10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35898,7 +35900,7 @@
       </c>
       <c r="H736" s="11"/>
       <c r="I736" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="737" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -35925,7 +35927,7 @@
       </c>
       <c r="H737" s="11"/>
       <c r="I737" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="738" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -35952,7 +35954,7 @@
       </c>
       <c r="H738" s="11"/>
       <c r="I738" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="739" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35979,7 +35981,7 @@
       </c>
       <c r="H739" s="11"/>
       <c r="I739" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="740" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -36006,7 +36008,7 @@
       </c>
       <c r="H740" s="11"/>
       <c r="I740" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="741" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -36033,7 +36035,7 @@
       </c>
       <c r="H741" s="11"/>
       <c r="I741" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="742" spans="1:9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -36060,7 +36062,7 @@
       </c>
       <c r="H742" s="11"/>
       <c r="I742" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="743" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -36087,7 +36089,7 @@
       </c>
       <c r="H743" s="11"/>
       <c r="I743" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="744" spans="1:9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -36896,7 +36898,7 @@
       </c>
       <c r="H793" s="11"/>
       <c r="I793" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="794" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -36923,7 +36925,7 @@
       </c>
       <c r="H794" s="11"/>
       <c r="I794" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="795" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -36950,7 +36952,7 @@
       </c>
       <c r="H795" s="11"/>
       <c r="I795" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="796" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -36977,7 +36979,7 @@
       </c>
       <c r="H796" s="11"/>
       <c r="I796" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="797" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -37004,7 +37006,7 @@
       </c>
       <c r="H797" s="11"/>
       <c r="I797" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="798" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -37031,7 +37033,7 @@
       </c>
       <c r="H798" s="11"/>
       <c r="I798" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="799" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -37154,7 +37156,7 @@
       </c>
       <c r="H805" s="11"/>
       <c r="I805" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="806" spans="1:9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -37523,11 +37525,11 @@
         <v>1310</v>
       </c>
       <c r="G828" s="18" t="s">
-        <v>7335</v>
+        <v>7334</v>
       </c>
       <c r="H828" s="53"/>
       <c r="I828" s="11" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="829" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -37544,11 +37546,11 @@
         <v>1539</v>
       </c>
       <c r="G829" s="18" t="s">
-        <v>7335</v>
+        <v>7334</v>
       </c>
       <c r="H829" s="53"/>
       <c r="I829" s="11" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="830" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -43459,11 +43461,11 @@
         <v>2322</v>
       </c>
       <c r="G1199" s="18" t="s">
-        <v>7339</v>
+        <v>7338</v>
       </c>
       <c r="H1199" s="11"/>
       <c r="I1199" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="1200" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -44894,7 +44896,7 @@
       </c>
       <c r="H1288" s="11"/>
       <c r="I1288" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="1289" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -46357,7 +46359,7 @@
       </c>
       <c r="H1379" s="11"/>
       <c r="I1379" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="1380" spans="1:9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -46374,11 +46376,11 @@
         <v>2851</v>
       </c>
       <c r="G1380" s="18" t="s">
-        <v>7335</v>
+        <v>7334</v>
       </c>
       <c r="H1380" s="53"/>
       <c r="I1380" s="11" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="1381" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -52213,7 +52215,7 @@
       </c>
       <c r="H1745" s="11"/>
       <c r="I1745" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="1746" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -52304,7 +52306,7 @@
       </c>
       <c r="H1750" s="11"/>
       <c r="I1750" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="1751" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -52983,11 +52985,11 @@
         <v>3672</v>
       </c>
       <c r="G1792" s="18" t="s">
-        <v>7351</v>
+        <v>7350</v>
       </c>
       <c r="H1792" s="11"/>
       <c r="I1792" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="1793" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -54082,7 +54084,7 @@
       </c>
       <c r="H1860" s="11"/>
       <c r="I1860" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="1861" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -54813,7 +54815,7 @@
       </c>
       <c r="H1905" s="11"/>
       <c r="I1905" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="1906" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -60804,7 +60806,7 @@
       </c>
       <c r="H2280" s="11"/>
       <c r="I2280" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="2281" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -63051,7 +63053,7 @@
       </c>
       <c r="H2420" s="11"/>
       <c r="I2420" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="2421" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -63782,7 +63784,7 @@
       </c>
       <c r="H2465" s="11"/>
       <c r="I2465" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="2466" spans="1:9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -82227,11 +82229,11 @@
         <v>751</v>
       </c>
       <c r="G3621" s="52" t="s">
-        <v>7335</v>
+        <v>7334</v>
       </c>
       <c r="H3621" s="53"/>
       <c r="I3621" s="11" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
delete enolisation (with wrong ID) in RXNO but
add "realizes some enolisability" subclassOf axiom in MOP and change genus in textual definition according to equivalentTo axiom.
</commit_message>
<xml_diff>
--- a/docs/#27_workfiles/MOP_vs_RXNO.xlsx
+++ b/docs/#27_workfiles/MOP_vs_RXNO.xlsx
@@ -22084,9 +22084,6 @@
     <t>use MOP version, as its parent is more precise</t>
   </si>
   <si>
-    <t>"enolization" is MOP:0000672 --&gt; wrong ID in RXNO; sync axioms and use MOP parent 'keto-enol tautomerisation'</t>
-  </si>
-  <si>
     <t>cut to MOP</t>
   </si>
   <si>
@@ -22175,6 +22172,9 @@
   </si>
   <si>
     <t>use RXNO version as its parent is more precise and drop equivalentTo Axiom in MOP</t>
+  </si>
+  <si>
+    <t>"enolization" is MOP:0000672 --&gt; wrong ID in RXNO; sync axioms and use MOP parent 'keto-enol tautomerisation' --&gt; thus change textual definition. Consider dropping equivalentTo axiom.</t>
   </si>
 </sst>
 </file>
@@ -23058,8 +23058,8 @@
   <dimension ref="A1:J3621"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A663" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E665" sqref="E665"/>
+      <pane ySplit="2" topLeftCell="A712" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G719" sqref="G719"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23095,7 +23095,7 @@
         <v>7314</v>
       </c>
       <c r="I1" t="s">
-        <v>7335</v>
+        <v>7334</v>
       </c>
     </row>
     <row r="2" spans="1:9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -23188,11 +23188,11 @@
         <v>15</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>7340</v>
+        <v>7339</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="7" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -28563,7 +28563,7 @@
       </c>
       <c r="H342" s="11"/>
       <c r="I342" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="343" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -28974,7 +28974,7 @@
       </c>
       <c r="H367" s="11"/>
       <c r="I367" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="368" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -29065,7 +29065,7 @@
       </c>
       <c r="H372" s="11"/>
       <c r="I372" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="373" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -29732,7 +29732,7 @@
       </c>
       <c r="H413" s="11"/>
       <c r="I413" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="414" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -29759,7 +29759,7 @@
       </c>
       <c r="H414" s="11"/>
       <c r="I414" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="415" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -29946,7 +29946,7 @@
       </c>
       <c r="H425" s="11"/>
       <c r="I425" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="426" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -30529,7 +30529,7 @@
       </c>
       <c r="H461" s="11"/>
       <c r="I461" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="462" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -30872,11 +30872,11 @@
         <v>72</v>
       </c>
       <c r="G482" s="18" t="s">
-        <v>7339</v>
+        <v>7338</v>
       </c>
       <c r="H482" s="11"/>
       <c r="I482" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="483" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -31597,7 +31597,7 @@
       <c r="G527" s="18"/>
       <c r="H527" s="11"/>
       <c r="I527" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="528" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -31848,7 +31848,7 @@
       </c>
       <c r="H542" s="11"/>
       <c r="I542" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="543" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -31923,7 +31923,7 @@
       </c>
       <c r="H546" s="11"/>
       <c r="I546" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="547" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32046,7 +32046,7 @@
       </c>
       <c r="H553" s="53"/>
       <c r="I553" s="11" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="554" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32137,7 +32137,7 @@
       </c>
       <c r="H558" s="11"/>
       <c r="I558" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="559" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -32160,11 +32160,11 @@
         <v>1144</v>
       </c>
       <c r="G559" s="18" t="s">
-        <v>7342</v>
+        <v>7341</v>
       </c>
       <c r="H559" s="11"/>
       <c r="I559" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="560" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -32255,7 +32255,7 @@
       </c>
       <c r="H564" s="11"/>
       <c r="I564" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="565" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32282,7 +32282,7 @@
       </c>
       <c r="H565" s="11"/>
       <c r="I565" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="566" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32309,7 +32309,7 @@
       </c>
       <c r="H566" s="11"/>
       <c r="I566" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="567" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32336,7 +32336,7 @@
       </c>
       <c r="H567" s="11"/>
       <c r="I567" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="568" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -32363,7 +32363,7 @@
       </c>
       <c r="H568" s="11"/>
       <c r="I568" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="569" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -32390,7 +32390,7 @@
       </c>
       <c r="H569" s="11"/>
       <c r="I569" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="570" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -32417,7 +32417,7 @@
       </c>
       <c r="H570" s="11"/>
       <c r="I570" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="571" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32444,7 +32444,7 @@
       </c>
       <c r="H571" s="11"/>
       <c r="I571" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="572" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32471,7 +32471,7 @@
       </c>
       <c r="H572" s="11"/>
       <c r="I572" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="573" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32498,7 +32498,7 @@
       </c>
       <c r="H573" s="11"/>
       <c r="I573" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="574" spans="1:9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -32518,14 +32518,14 @@
         <v>1178</v>
       </c>
       <c r="F574" s="54" t="s">
-        <v>7344</v>
+        <v>7343</v>
       </c>
       <c r="G574" s="18" t="s">
         <v>7324</v>
       </c>
       <c r="H574" s="11"/>
       <c r="I574" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="575" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -32545,14 +32545,14 @@
         <v>1180</v>
       </c>
       <c r="F575" s="54" t="s">
-        <v>7343</v>
+        <v>7342</v>
       </c>
       <c r="G575" s="18" t="s">
         <v>7325</v>
       </c>
       <c r="H575" s="11"/>
       <c r="I575" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="576" spans="1:9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -32579,7 +32579,7 @@
       </c>
       <c r="H576" s="11"/>
       <c r="I576" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="577" spans="1:9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -32599,14 +32599,14 @@
         <v>1187</v>
       </c>
       <c r="F577" s="54" t="s">
-        <v>7345</v>
+        <v>7344</v>
       </c>
       <c r="G577" s="18" t="s">
         <v>7326</v>
       </c>
       <c r="H577" s="11"/>
       <c r="I577" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="578" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32633,7 +32633,7 @@
       </c>
       <c r="H578" s="11"/>
       <c r="I578" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="579" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32660,7 +32660,7 @@
       </c>
       <c r="H579" s="11"/>
       <c r="I579" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="580" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -32680,14 +32680,14 @@
         <v>1194</v>
       </c>
       <c r="F580" s="54" t="s">
-        <v>7346</v>
+        <v>7345</v>
       </c>
       <c r="G580" s="18" t="s">
         <v>7325</v>
       </c>
       <c r="H580" s="11"/>
       <c r="I580" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="581" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -32707,14 +32707,14 @@
         <v>1196</v>
       </c>
       <c r="F581" s="54" t="s">
-        <v>7347</v>
+        <v>7346</v>
       </c>
       <c r="G581" s="18" t="s">
         <v>7325</v>
       </c>
       <c r="H581" s="11"/>
       <c r="I581" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="582" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -32734,14 +32734,14 @@
         <v>1198</v>
       </c>
       <c r="F582" s="54" t="s">
-        <v>7348</v>
+        <v>7347</v>
       </c>
       <c r="G582" s="18" t="s">
         <v>7325</v>
       </c>
       <c r="H582" s="11"/>
       <c r="I582" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="583" spans="1:9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -32761,14 +32761,14 @@
         <v>1200</v>
       </c>
       <c r="F583" s="54" t="s">
-        <v>7349</v>
+        <v>7348</v>
       </c>
       <c r="G583" s="18" t="s">
         <v>7324</v>
       </c>
       <c r="H583" s="11"/>
       <c r="I583" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="584" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -32795,7 +32795,7 @@
       </c>
       <c r="H584" s="11"/>
       <c r="I584" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="585" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -32822,7 +32822,7 @@
       </c>
       <c r="H585" s="11"/>
       <c r="I585" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="586" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -32849,7 +32849,7 @@
       </c>
       <c r="H586" s="11"/>
       <c r="I586" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="587" spans="1:9" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
@@ -32872,11 +32872,11 @@
         <v>1211</v>
       </c>
       <c r="G587" s="35" t="s">
-        <v>7354</v>
+        <v>7353</v>
       </c>
       <c r="H587" s="11"/>
       <c r="I587" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="588" spans="1:9" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -32899,11 +32899,11 @@
         <v>1214</v>
       </c>
       <c r="G588" s="35" t="s">
-        <v>7354</v>
+        <v>7353</v>
       </c>
       <c r="H588" s="11"/>
       <c r="I588" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="589" spans="1:9" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -32926,11 +32926,11 @@
         <v>1217</v>
       </c>
       <c r="G589" s="35" t="s">
-        <v>7354</v>
+        <v>7353</v>
       </c>
       <c r="H589" s="11"/>
       <c r="I589" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="590" spans="1:9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -32953,11 +32953,11 @@
         <v>1220</v>
       </c>
       <c r="G590" s="35" t="s">
-        <v>7354</v>
+        <v>7353</v>
       </c>
       <c r="H590" s="11"/>
       <c r="I590" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="591" spans="1:9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -32980,11 +32980,11 @@
         <v>1214</v>
       </c>
       <c r="G591" s="35" t="s">
-        <v>7354</v>
+        <v>7353</v>
       </c>
       <c r="H591" s="11"/>
       <c r="I591" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="592" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33011,7 +33011,7 @@
       </c>
       <c r="H592" s="11"/>
       <c r="I592" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="593" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33030,7 +33030,7 @@
       <c r="G593" s="18"/>
       <c r="H593" s="11"/>
       <c r="I593" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="594" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33049,7 +33049,7 @@
       <c r="G594" s="18"/>
       <c r="H594" s="11"/>
       <c r="I594" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="595" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33068,7 +33068,7 @@
       <c r="G595" s="18"/>
       <c r="H595" s="11"/>
       <c r="I595" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="596" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33087,7 +33087,7 @@
       <c r="G596" s="18"/>
       <c r="H596" s="11"/>
       <c r="I596" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="597" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33106,7 +33106,7 @@
       <c r="G597" s="18"/>
       <c r="H597" s="11"/>
       <c r="I597" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="598" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33125,7 +33125,7 @@
       <c r="G598" s="18"/>
       <c r="H598" s="11"/>
       <c r="I598" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="599" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -33152,7 +33152,7 @@
       </c>
       <c r="H599" s="11"/>
       <c r="I599" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="600" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -33171,7 +33171,7 @@
       <c r="G600" s="18"/>
       <c r="H600" s="11"/>
       <c r="I600" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="601" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -33190,7 +33190,7 @@
       <c r="G601" s="18"/>
       <c r="H601" s="11"/>
       <c r="I601" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="602" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -33209,7 +33209,7 @@
       <c r="G602" s="18"/>
       <c r="H602" s="11"/>
       <c r="I602" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="603" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -33228,7 +33228,7 @@
       <c r="G603" s="18"/>
       <c r="H603" s="11"/>
       <c r="I603" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="604" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -33247,7 +33247,7 @@
       <c r="G604" s="18"/>
       <c r="H604" s="11"/>
       <c r="I604" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="605" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -33266,7 +33266,7 @@
       <c r="G605" s="18"/>
       <c r="H605" s="11"/>
       <c r="I605" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="606" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -33285,7 +33285,7 @@
       <c r="G606" s="18"/>
       <c r="H606" s="11"/>
       <c r="I606" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="607" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33304,7 +33304,7 @@
       <c r="G607" s="18"/>
       <c r="H607" s="11"/>
       <c r="I607" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="608" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33323,7 +33323,7 @@
       <c r="G608" s="18"/>
       <c r="H608" s="11"/>
       <c r="I608" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="609" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33342,7 +33342,7 @@
       <c r="G609" s="18"/>
       <c r="H609" s="11"/>
       <c r="I609" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="610" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33361,7 +33361,7 @@
       <c r="G610" s="18"/>
       <c r="H610" s="11"/>
       <c r="I610" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="611" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33380,7 +33380,7 @@
       <c r="G611" s="18"/>
       <c r="H611" s="11"/>
       <c r="I611" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="612" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33399,7 +33399,7 @@
       <c r="G612" s="18"/>
       <c r="H612" s="11"/>
       <c r="I612" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="613" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33418,7 +33418,7 @@
       <c r="G613" s="18"/>
       <c r="H613" s="11"/>
       <c r="I613" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="614" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33437,7 +33437,7 @@
       <c r="G614" s="18"/>
       <c r="H614" s="11"/>
       <c r="I614" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="615" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33456,7 +33456,7 @@
       <c r="G615" s="18"/>
       <c r="H615" s="11"/>
       <c r="I615" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="616" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -33475,7 +33475,7 @@
       <c r="G616" s="18"/>
       <c r="H616" s="11"/>
       <c r="I616" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="617" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33494,7 +33494,7 @@
       <c r="G617" s="18"/>
       <c r="H617" s="11"/>
       <c r="I617" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="618" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33513,7 +33513,7 @@
       <c r="G618" s="18"/>
       <c r="H618" s="11"/>
       <c r="I618" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="619" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -33532,7 +33532,7 @@
       <c r="G619" s="18"/>
       <c r="H619" s="11"/>
       <c r="I619" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="620" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -33551,7 +33551,7 @@
       <c r="G620" s="18"/>
       <c r="H620" s="11"/>
       <c r="I620" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="621" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33578,7 +33578,7 @@
       </c>
       <c r="H621" s="11"/>
       <c r="I621" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="622" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33605,7 +33605,7 @@
       </c>
       <c r="H622" s="11"/>
       <c r="I622" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="623" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33624,7 +33624,7 @@
       <c r="G623" s="18"/>
       <c r="H623" s="11"/>
       <c r="I623" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="624" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33643,7 +33643,7 @@
       <c r="G624" s="18"/>
       <c r="H624" s="11"/>
       <c r="I624" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="625" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33662,7 +33662,7 @@
       <c r="G625" s="18"/>
       <c r="H625" s="11"/>
       <c r="I625" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="626" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33681,7 +33681,7 @@
       <c r="G626" s="18"/>
       <c r="H626" s="11"/>
       <c r="I626" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="627" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33700,7 +33700,7 @@
       <c r="G627" s="18"/>
       <c r="H627" s="11"/>
       <c r="I627" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="628" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33719,7 +33719,7 @@
       <c r="G628" s="18"/>
       <c r="H628" s="11"/>
       <c r="I628" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="629" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33738,7 +33738,7 @@
       <c r="G629" s="18"/>
       <c r="H629" s="11"/>
       <c r="I629" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="630" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -33765,7 +33765,7 @@
       </c>
       <c r="H630" s="11"/>
       <c r="I630" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="631" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -33792,7 +33792,7 @@
       </c>
       <c r="H631" s="11"/>
       <c r="I631" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="632" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -33811,7 +33811,7 @@
       <c r="G632" s="18"/>
       <c r="H632" s="11"/>
       <c r="I632" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="633" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33830,7 +33830,7 @@
       <c r="G633" s="18"/>
       <c r="H633" s="11"/>
       <c r="I633" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="634" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -33849,7 +33849,7 @@
       <c r="G634" s="18"/>
       <c r="H634" s="11"/>
       <c r="I634" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="635" spans="1:9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -33868,7 +33868,7 @@
       <c r="G635" s="18"/>
       <c r="H635" s="11"/>
       <c r="I635" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="636" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -33887,7 +33887,7 @@
       <c r="G636" s="18"/>
       <c r="H636" s="11"/>
       <c r="I636" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="637" spans="1:9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -33906,7 +33906,7 @@
       <c r="G637" s="18"/>
       <c r="H637" s="11"/>
       <c r="I637" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="638" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33925,7 +33925,7 @@
       <c r="G638" s="18"/>
       <c r="H638" s="11"/>
       <c r="I638" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="639" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -33944,7 +33944,7 @@
       <c r="G639" s="18"/>
       <c r="H639" s="11"/>
       <c r="I639" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="640" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -33963,7 +33963,7 @@
       <c r="G640" s="18"/>
       <c r="H640" s="11"/>
       <c r="I640" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="641" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -33982,7 +33982,7 @@
       <c r="G641" s="18"/>
       <c r="H641" s="11"/>
       <c r="I641" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="642" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -34001,7 +34001,7 @@
       <c r="G642" s="18"/>
       <c r="H642" s="11"/>
       <c r="I642" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="643" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -34020,7 +34020,7 @@
       <c r="G643" s="18"/>
       <c r="H643" s="11"/>
       <c r="I643" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="644" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -34039,7 +34039,7 @@
       <c r="G644" s="18"/>
       <c r="H644" s="11"/>
       <c r="I644" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="645" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -34066,7 +34066,7 @@
       </c>
       <c r="H645" s="11"/>
       <c r="I645" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="646" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -34085,7 +34085,7 @@
       <c r="G646" s="18"/>
       <c r="H646" s="11"/>
       <c r="I646" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="647" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -34104,7 +34104,7 @@
       <c r="G647" s="18"/>
       <c r="H647" s="11"/>
       <c r="I647" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="648" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -34123,7 +34123,7 @@
       <c r="G648" s="18"/>
       <c r="H648" s="11"/>
       <c r="I648" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="649" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -34142,7 +34142,7 @@
       <c r="G649" s="18"/>
       <c r="H649" s="11"/>
       <c r="I649" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="650" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -34161,7 +34161,7 @@
       <c r="G650" s="18"/>
       <c r="H650" s="11"/>
       <c r="I650" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="651" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -34180,7 +34180,7 @@
       <c r="G651" s="18"/>
       <c r="H651" s="11"/>
       <c r="I651" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="652" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -34199,7 +34199,7 @@
       <c r="G652" s="18"/>
       <c r="H652" s="11"/>
       <c r="I652" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="653" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -34226,7 +34226,7 @@
       </c>
       <c r="H653" s="11"/>
       <c r="I653" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="654" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -34245,7 +34245,7 @@
       <c r="G654" s="18"/>
       <c r="H654" s="11"/>
       <c r="I654" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="655" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -34264,7 +34264,7 @@
       <c r="G655" s="18"/>
       <c r="H655" s="11"/>
       <c r="I655" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="656" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -34283,7 +34283,7 @@
       <c r="G656" s="18"/>
       <c r="H656" s="11"/>
       <c r="I656" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="657" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -34302,7 +34302,7 @@
       <c r="G657" s="18"/>
       <c r="H657" s="11"/>
       <c r="I657" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="658" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -34321,7 +34321,7 @@
       <c r="G658" s="18"/>
       <c r="H658" s="11"/>
       <c r="I658" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="659" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -34348,7 +34348,7 @@
       </c>
       <c r="H659" s="11"/>
       <c r="I659" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="660" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -34367,7 +34367,7 @@
       <c r="G660" s="18"/>
       <c r="H660" s="11"/>
       <c r="I660" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="661" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -34386,7 +34386,7 @@
       <c r="G661" s="18"/>
       <c r="H661" s="11"/>
       <c r="I661" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="662" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -34405,7 +34405,7 @@
       <c r="G662" s="18"/>
       <c r="H662" s="11"/>
       <c r="I662" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="663" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -34424,7 +34424,7 @@
       <c r="G663" s="18"/>
       <c r="H663" s="11"/>
       <c r="I663" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="664" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -34443,7 +34443,7 @@
       <c r="G664" s="18"/>
       <c r="H664" s="11"/>
       <c r="I664" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="665" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -34462,7 +34462,7 @@
       <c r="G665" s="18"/>
       <c r="H665" s="11"/>
       <c r="I665" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="666" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -34481,7 +34481,7 @@
       <c r="G666" s="18"/>
       <c r="H666" s="11"/>
       <c r="I666" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="667" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -34500,7 +34500,7 @@
       <c r="G667" s="18"/>
       <c r="H667" s="11"/>
       <c r="I667" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="668" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -34519,7 +34519,7 @@
       <c r="G668" s="18"/>
       <c r="H668" s="11"/>
       <c r="I668" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="669" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -34538,7 +34538,7 @@
       <c r="G669" s="18"/>
       <c r="H669" s="11"/>
       <c r="I669" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="670" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -34557,7 +34557,7 @@
       <c r="G670" s="18"/>
       <c r="H670" s="11"/>
       <c r="I670" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="671" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -34576,7 +34576,7 @@
       <c r="G671" s="18"/>
       <c r="H671" s="11"/>
       <c r="I671" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="672" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -34595,7 +34595,7 @@
       <c r="G672" s="18"/>
       <c r="H672" s="11"/>
       <c r="I672" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="673" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -34614,7 +34614,7 @@
       <c r="G673" s="18"/>
       <c r="H673" s="11"/>
       <c r="I673" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="674" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -34637,11 +34637,11 @@
         <v>1415</v>
       </c>
       <c r="G674" s="18" t="s">
-        <v>7358</v>
+        <v>7357</v>
       </c>
       <c r="H674" s="11"/>
       <c r="I674" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="675" spans="1:9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -34661,12 +34661,12 @@
         <v>1417</v>
       </c>
       <c r="F675" s="55" t="s">
-        <v>7351</v>
+        <v>7350</v>
       </c>
       <c r="G675" s="18"/>
       <c r="H675" s="11"/>
       <c r="I675" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="676" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -34685,7 +34685,7 @@
       <c r="G676" s="18"/>
       <c r="H676" s="11"/>
       <c r="I676" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="677" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -34704,7 +34704,7 @@
       <c r="G677" s="18"/>
       <c r="H677" s="11"/>
       <c r="I677" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="678" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -34723,7 +34723,7 @@
       <c r="G678" s="18"/>
       <c r="H678" s="11"/>
       <c r="I678" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="679" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -34742,7 +34742,7 @@
       <c r="G679" s="18"/>
       <c r="H679" s="11"/>
       <c r="I679" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="680" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -34761,7 +34761,7 @@
       <c r="G680" s="18"/>
       <c r="H680" s="11"/>
       <c r="I680" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="681" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -34780,7 +34780,7 @@
       <c r="G681" s="18"/>
       <c r="H681" s="11"/>
       <c r="I681" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="682" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -34799,7 +34799,7 @@
       <c r="G682" s="18"/>
       <c r="H682" s="11"/>
       <c r="I682" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="683" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -34818,7 +34818,7 @@
       <c r="G683" s="18"/>
       <c r="H683" s="11"/>
       <c r="I683" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="684" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -34837,7 +34837,7 @@
       <c r="G684" s="18"/>
       <c r="H684" s="11"/>
       <c r="I684" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="685" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -34856,7 +34856,7 @@
       <c r="G685" s="18"/>
       <c r="H685" s="11"/>
       <c r="I685" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="686" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -34875,7 +34875,7 @@
       <c r="G686" s="18"/>
       <c r="H686" s="11"/>
       <c r="I686" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="687" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -34894,7 +34894,7 @@
       <c r="G687" s="18"/>
       <c r="H687" s="11"/>
       <c r="I687" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="688" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -34913,7 +34913,7 @@
       <c r="G688" s="18"/>
       <c r="H688" s="11"/>
       <c r="I688" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="689" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -34932,7 +34932,7 @@
       <c r="G689" s="18"/>
       <c r="H689" s="11"/>
       <c r="I689" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="690" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -34951,7 +34951,7 @@
       <c r="G690" s="18"/>
       <c r="H690" s="11"/>
       <c r="I690" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="691" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -34970,7 +34970,7 @@
       <c r="G691" s="18"/>
       <c r="H691" s="11"/>
       <c r="I691" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="692" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -34989,7 +34989,7 @@
       <c r="G692" s="18"/>
       <c r="H692" s="11"/>
       <c r="I692" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="693" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -35008,7 +35008,7 @@
       <c r="G693" s="18"/>
       <c r="H693" s="11"/>
       <c r="I693" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="694" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -35027,7 +35027,7 @@
       <c r="G694" s="18"/>
       <c r="H694" s="11"/>
       <c r="I694" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="695" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -35046,7 +35046,7 @@
       <c r="G695" s="18"/>
       <c r="H695" s="11"/>
       <c r="I695" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="696" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35065,7 +35065,7 @@
       <c r="G696" s="18"/>
       <c r="H696" s="11"/>
       <c r="I696" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="697" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35084,7 +35084,7 @@
       <c r="G697" s="18"/>
       <c r="H697" s="11"/>
       <c r="I697" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="698" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35103,7 +35103,7 @@
       <c r="G698" s="18"/>
       <c r="H698" s="11"/>
       <c r="I698" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="699" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35122,7 +35122,7 @@
       <c r="G699" s="18"/>
       <c r="H699" s="11"/>
       <c r="I699" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="700" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35141,7 +35141,7 @@
       <c r="G700" s="18"/>
       <c r="H700" s="11"/>
       <c r="I700" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="701" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35160,7 +35160,7 @@
       <c r="G701" s="18"/>
       <c r="H701" s="11"/>
       <c r="I701" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="702" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35179,7 +35179,7 @@
       <c r="G702" s="18"/>
       <c r="H702" s="11"/>
       <c r="I702" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="703" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35198,7 +35198,7 @@
       <c r="G703" s="18"/>
       <c r="H703" s="11"/>
       <c r="I703" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="704" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35217,7 +35217,7 @@
       <c r="G704" s="18"/>
       <c r="H704" s="11"/>
       <c r="I704" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="705" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35236,7 +35236,7 @@
       <c r="G705" s="18"/>
       <c r="H705" s="11"/>
       <c r="I705" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="706" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -35255,7 +35255,7 @@
       <c r="G706" s="18"/>
       <c r="H706" s="11"/>
       <c r="I706" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="707" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -35274,7 +35274,7 @@
       <c r="G707" s="18"/>
       <c r="H707" s="11"/>
       <c r="I707" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="708" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -35301,7 +35301,7 @@
       </c>
       <c r="H708" s="11"/>
       <c r="I708" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="709" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -35328,7 +35328,7 @@
       </c>
       <c r="H709" s="11"/>
       <c r="I709" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="710" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -35361,7 +35361,7 @@
       <c r="E711" s="27"/>
       <c r="F711" s="9"/>
       <c r="G711" s="35" t="s">
-        <v>7353</v>
+        <v>7352</v>
       </c>
       <c r="H711" s="11"/>
     </row>
@@ -35433,11 +35433,11 @@
         <v>1521</v>
       </c>
       <c r="G715" s="18" t="s">
-        <v>7352</v>
+        <v>7351</v>
       </c>
       <c r="H715" s="11"/>
       <c r="I715" s="11" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="716" spans="1:9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -35460,11 +35460,11 @@
         <v>1524</v>
       </c>
       <c r="G716" s="18" t="s">
-        <v>7355</v>
+        <v>7354</v>
       </c>
       <c r="H716" s="11"/>
       <c r="I716" s="11" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="717" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35487,11 +35487,11 @@
         <v>1172</v>
       </c>
       <c r="G717" s="18" t="s">
-        <v>7356</v>
+        <v>7355</v>
       </c>
       <c r="H717" s="11"/>
       <c r="I717" s="11" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="718" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -35514,11 +35514,11 @@
         <v>1158</v>
       </c>
       <c r="G718" s="18" t="s">
-        <v>7357</v>
+        <v>7356</v>
       </c>
       <c r="H718" s="11"/>
       <c r="I718" s="11" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="719" spans="1:9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -35541,11 +35541,11 @@
         <v>1536</v>
       </c>
       <c r="G719" s="18" t="s">
-        <v>7333</v>
+        <v>7358</v>
       </c>
       <c r="H719" s="11"/>
       <c r="I719" s="11" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="720" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -35562,11 +35562,11 @@
         <v>1539</v>
       </c>
       <c r="G720" s="18" t="s">
-        <v>7334</v>
+        <v>7333</v>
       </c>
       <c r="H720" s="53"/>
       <c r="I720" s="11" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="721" spans="1:10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -35583,11 +35583,11 @@
         <v>1542</v>
       </c>
       <c r="G721" s="18" t="s">
-        <v>7334</v>
+        <v>7333</v>
       </c>
       <c r="H721" s="53"/>
       <c r="I721" s="11" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="722" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
@@ -35604,11 +35604,11 @@
         <v>1545</v>
       </c>
       <c r="G722" s="18" t="s">
-        <v>7334</v>
+        <v>7333</v>
       </c>
       <c r="H722" s="53"/>
       <c r="I722" s="11" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="723" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
@@ -35625,11 +35625,11 @@
         <v>1158</v>
       </c>
       <c r="G723" s="18" t="s">
-        <v>7334</v>
+        <v>7333</v>
       </c>
       <c r="H723" s="53"/>
       <c r="I723" s="11" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="724" spans="1:10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -35652,14 +35652,14 @@
         <v>1115</v>
       </c>
       <c r="G724" s="18" t="s">
-        <v>7337</v>
+        <v>7336</v>
       </c>
       <c r="H724" s="11"/>
       <c r="I724" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
       <c r="J724" s="44" t="s">
-        <v>7336</v>
+        <v>7335</v>
       </c>
     </row>
     <row r="725" spans="1:10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35676,11 +35676,11 @@
         <v>1553</v>
       </c>
       <c r="G725" s="18" t="s">
-        <v>7334</v>
+        <v>7333</v>
       </c>
       <c r="H725" s="53"/>
       <c r="I725" s="11" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="726" spans="1:10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -35697,11 +35697,11 @@
         <v>1556</v>
       </c>
       <c r="G726" s="18" t="s">
-        <v>7334</v>
+        <v>7333</v>
       </c>
       <c r="H726" s="53"/>
       <c r="I726" s="11" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="727" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
@@ -35824,7 +35824,7 @@
       </c>
       <c r="H733" s="11"/>
       <c r="I733" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="734" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
@@ -35851,7 +35851,7 @@
       </c>
       <c r="H734" s="11"/>
       <c r="I734" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="735" spans="1:10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35878,7 +35878,7 @@
       </c>
       <c r="H735" s="11"/>
       <c r="I735" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="736" spans="1:10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35905,7 +35905,7 @@
       </c>
       <c r="H736" s="11"/>
       <c r="I736" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="737" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -35932,7 +35932,7 @@
       </c>
       <c r="H737" s="11"/>
       <c r="I737" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="738" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -35959,7 +35959,7 @@
       </c>
       <c r="H738" s="11"/>
       <c r="I738" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="739" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -35986,7 +35986,7 @@
       </c>
       <c r="H739" s="11"/>
       <c r="I739" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="740" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -36013,7 +36013,7 @@
       </c>
       <c r="H740" s="11"/>
       <c r="I740" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="741" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -36040,7 +36040,7 @@
       </c>
       <c r="H741" s="11"/>
       <c r="I741" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="742" spans="1:9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -36067,7 +36067,7 @@
       </c>
       <c r="H742" s="11"/>
       <c r="I742" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="743" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -36094,7 +36094,7 @@
       </c>
       <c r="H743" s="11"/>
       <c r="I743" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="744" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -36903,7 +36903,7 @@
       </c>
       <c r="H793" s="11"/>
       <c r="I793" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="794" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -36930,7 +36930,7 @@
       </c>
       <c r="H794" s="11"/>
       <c r="I794" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="795" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -36957,7 +36957,7 @@
       </c>
       <c r="H795" s="11"/>
       <c r="I795" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="796" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -36984,7 +36984,7 @@
       </c>
       <c r="H796" s="11"/>
       <c r="I796" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="797" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -37011,7 +37011,7 @@
       </c>
       <c r="H797" s="11"/>
       <c r="I797" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="798" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -37038,7 +37038,7 @@
       </c>
       <c r="H798" s="11"/>
       <c r="I798" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="799" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -37161,7 +37161,7 @@
       </c>
       <c r="H805" s="11"/>
       <c r="I805" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="806" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -37530,11 +37530,11 @@
         <v>1310</v>
       </c>
       <c r="G828" s="18" t="s">
-        <v>7334</v>
+        <v>7333</v>
       </c>
       <c r="H828" s="53"/>
       <c r="I828" s="11" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="829" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -37551,11 +37551,11 @@
         <v>1539</v>
       </c>
       <c r="G829" s="18" t="s">
-        <v>7334</v>
+        <v>7333</v>
       </c>
       <c r="H829" s="53"/>
       <c r="I829" s="11" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="830" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -43466,11 +43466,11 @@
         <v>2322</v>
       </c>
       <c r="G1199" s="18" t="s">
-        <v>7338</v>
+        <v>7337</v>
       </c>
       <c r="H1199" s="11"/>
       <c r="I1199" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="1200" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -44901,7 +44901,7 @@
       </c>
       <c r="H1288" s="11"/>
       <c r="I1288" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="1289" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -46364,7 +46364,7 @@
       </c>
       <c r="H1379" s="11"/>
       <c r="I1379" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="1380" spans="1:9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -46381,11 +46381,11 @@
         <v>2851</v>
       </c>
       <c r="G1380" s="18" t="s">
-        <v>7334</v>
+        <v>7333</v>
       </c>
       <c r="H1380" s="53"/>
       <c r="I1380" s="11" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="1381" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -52220,7 +52220,7 @@
       </c>
       <c r="H1745" s="11"/>
       <c r="I1745" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="1746" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -52311,7 +52311,7 @@
       </c>
       <c r="H1750" s="11"/>
       <c r="I1750" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="1751" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -52990,11 +52990,11 @@
         <v>3672</v>
       </c>
       <c r="G1792" s="18" t="s">
-        <v>7350</v>
+        <v>7349</v>
       </c>
       <c r="H1792" s="11"/>
       <c r="I1792" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="1793" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
@@ -54089,7 +54089,7 @@
       </c>
       <c r="H1860" s="11"/>
       <c r="I1860" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="1861" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -54820,7 +54820,7 @@
       </c>
       <c r="H1905" s="11"/>
       <c r="I1905" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="1906" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -60811,7 +60811,7 @@
       </c>
       <c r="H2280" s="11"/>
       <c r="I2280" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="2281" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -63058,7 +63058,7 @@
       </c>
       <c r="H2420" s="11"/>
       <c r="I2420" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="2421" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -63789,7 +63789,7 @@
       </c>
       <c r="H2465" s="11"/>
       <c r="I2465" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="2466" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -82234,11 +82234,11 @@
         <v>751</v>
       </c>
       <c r="G3621" s="52" t="s">
-        <v>7334</v>
+        <v>7333</v>
       </c>
       <c r="H3621" s="53"/>
       <c r="I3621" s="11" t="s">
-        <v>7341</v>
+        <v>7340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>